<commit_message>
Update project setting as to the new Spine model design
</commit_message>
<xml_diff>
--- a/spine_rts-gmlc/datasets/branch.xlsx
+++ b/spine_rts-gmlc/datasets/branch.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HJY_projects\spine\toolbox\projects\spine_rts-gmlc\.spinetoolbox\items\data_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HJY_projects\spine\RTS-GMLC_system_test\spinetoolbox_rts-gmlc\spine_rts-gmlc\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="branch" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="341">
   <si>
     <t>UID</t>
   </si>
@@ -781,9 +781,6 @@
     <t>node__temporal_block</t>
   </si>
   <si>
-    <t>conn_capacity</t>
-  </si>
-  <si>
     <t>RES_gen-212_CSP_1</t>
   </si>
   <si>
@@ -1033,9 +1030,6 @@
     <t>connection__node</t>
   </si>
   <si>
-    <t>fix_ratio_out_in_trans</t>
-  </si>
-  <si>
     <t>in_stor</t>
   </si>
   <si>
@@ -1049,6 +1043,12 @@
   </si>
   <si>
     <t>blk_t2</t>
+  </si>
+  <si>
+    <t>connection_capacity</t>
+  </si>
+  <si>
+    <t>fix_ratio_out_in_connection_flow</t>
   </si>
 </sst>
 </file>
@@ -11197,34 +11197,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>141</v>
       </c>
       <c r="B1" t="s">
         <v>142</v>
       </c>
-      <c r="C1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -11232,7 +11227,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -11240,7 +11235,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -11248,7 +11243,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>135</v>
       </c>
@@ -11256,7 +11251,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>135</v>
       </c>
@@ -11264,20 +11259,20 @@
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>135</v>
       </c>
       <c r="B7" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>135</v>
       </c>
       <c r="B8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -11289,8 +11284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11342,7 +11337,7 @@
         <v>148</v>
       </c>
       <c r="E2" t="s">
-        <v>251</v>
+        <v>339</v>
       </c>
       <c r="F2">
         <v>175</v>
@@ -11362,7 +11357,7 @@
         <v>149</v>
       </c>
       <c r="E3" t="s">
-        <v>251</v>
+        <v>339</v>
       </c>
       <c r="F3">
         <v>175</v>
@@ -11382,7 +11377,7 @@
         <v>148</v>
       </c>
       <c r="E4" t="s">
-        <v>251</v>
+        <v>339</v>
       </c>
       <c r="F4">
         <v>175</v>
@@ -11402,7 +11397,7 @@
         <v>149</v>
       </c>
       <c r="E5" t="s">
-        <v>251</v>
+        <v>339</v>
       </c>
       <c r="F5">
         <v>175</v>
@@ -11422,7 +11417,7 @@
         <v>148</v>
       </c>
       <c r="E6" t="s">
-        <v>251</v>
+        <v>339</v>
       </c>
       <c r="F6">
         <v>500</v>
@@ -11442,7 +11437,7 @@
         <v>149</v>
       </c>
       <c r="E7" t="s">
-        <v>251</v>
+        <v>339</v>
       </c>
       <c r="F7">
         <v>500</v>
@@ -11462,7 +11457,7 @@
         <v>148</v>
       </c>
       <c r="E8" t="s">
-        <v>251</v>
+        <v>339</v>
       </c>
       <c r="F8">
         <v>500</v>
@@ -11482,7 +11477,7 @@
         <v>149</v>
       </c>
       <c r="E9" t="s">
-        <v>251</v>
+        <v>339</v>
       </c>
       <c r="F9">
         <v>500</v>
@@ -11502,7 +11497,7 @@
         <v>148</v>
       </c>
       <c r="E10" t="s">
-        <v>251</v>
+        <v>339</v>
       </c>
       <c r="F10">
         <v>500</v>
@@ -11522,7 +11517,7 @@
         <v>149</v>
       </c>
       <c r="E11" t="s">
-        <v>251</v>
+        <v>339</v>
       </c>
       <c r="F11">
         <v>500</v>
@@ -11542,7 +11537,7 @@
         <v>148</v>
       </c>
       <c r="E12" t="s">
-        <v>251</v>
+        <v>339</v>
       </c>
       <c r="F12">
         <v>500</v>
@@ -11562,7 +11557,7 @@
         <v>149</v>
       </c>
       <c r="E13" t="s">
-        <v>251</v>
+        <v>339</v>
       </c>
       <c r="F13">
         <v>500</v>
@@ -11582,7 +11577,7 @@
         <v>148</v>
       </c>
       <c r="E14" t="s">
-        <v>251</v>
+        <v>339</v>
       </c>
       <c r="F14">
         <v>500</v>
@@ -11602,7 +11597,7 @@
         <v>149</v>
       </c>
       <c r="E15" t="s">
-        <v>251</v>
+        <v>339</v>
       </c>
       <c r="F15">
         <v>500</v>
@@ -11622,7 +11617,7 @@
         <v>148</v>
       </c>
       <c r="E16" t="s">
-        <v>251</v>
+        <v>339</v>
       </c>
       <c r="F16">
         <v>500</v>
@@ -11642,7 +11637,7 @@
         <v>149</v>
       </c>
       <c r="E17" t="s">
-        <v>251</v>
+        <v>339</v>
       </c>
       <c r="F17">
         <v>500</v>
@@ -11662,7 +11657,7 @@
         <v>148</v>
       </c>
       <c r="E18" t="s">
-        <v>251</v>
+        <v>339</v>
       </c>
       <c r="F18">
         <v>500</v>
@@ -11682,7 +11677,7 @@
         <v>149</v>
       </c>
       <c r="E19" t="s">
-        <v>251</v>
+        <v>339</v>
       </c>
       <c r="F19">
         <v>500</v>
@@ -11702,7 +11697,7 @@
         <v>148</v>
       </c>
       <c r="E20" t="s">
-        <v>251</v>
+        <v>339</v>
       </c>
       <c r="F20">
         <v>500</v>
@@ -11722,7 +11717,7 @@
         <v>149</v>
       </c>
       <c r="E21" t="s">
-        <v>251</v>
+        <v>339</v>
       </c>
       <c r="F21">
         <v>500</v>
@@ -11733,10 +11728,10 @@
         <v>140</v>
       </c>
       <c r="B22" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C22" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D22" t="s">
         <v>148</v>
@@ -11747,10 +11742,10 @@
         <v>140</v>
       </c>
       <c r="B23" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C23" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D23" t="s">
         <v>149</v>
@@ -11849,15 +11844,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="5" max="5" width="29.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -11882,7 +11877,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>243</v>
@@ -11894,7 +11889,7 @@
         <v>147</v>
       </c>
       <c r="E2" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="F2">
         <v>0.99</v>
@@ -11902,7 +11897,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>244</v>
@@ -11914,7 +11909,7 @@
         <v>147</v>
       </c>
       <c r="E3" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="F3">
         <v>0.99</v>
@@ -11922,7 +11917,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>245</v>
@@ -11934,7 +11929,7 @@
         <v>147</v>
       </c>
       <c r="E4" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="F4">
         <v>0.99</v>
@@ -11942,7 +11937,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>144</v>
@@ -11954,7 +11949,7 @@
         <v>150</v>
       </c>
       <c r="E5" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="F5">
         <v>0.99</v>
@@ -11962,7 +11957,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>145</v>
@@ -11974,7 +11969,7 @@
         <v>150</v>
       </c>
       <c r="E6" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="F6">
         <v>0.99</v>
@@ -11982,7 +11977,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>243</v>
@@ -11994,7 +11989,7 @@
         <v>146</v>
       </c>
       <c r="E7" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="F7">
         <v>0.99</v>
@@ -12002,7 +11997,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>244</v>
@@ -12014,7 +12009,7 @@
         <v>146</v>
       </c>
       <c r="E8" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="F8">
         <v>0.99</v>
@@ -12022,7 +12017,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>245</v>
@@ -12034,7 +12029,7 @@
         <v>146</v>
       </c>
       <c r="E9" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="F9">
         <v>0.99</v>
@@ -12042,7 +12037,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>144</v>
@@ -12054,7 +12049,7 @@
         <v>146</v>
       </c>
       <c r="E10" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="F10">
         <v>0.99</v>
@@ -12062,7 +12057,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>145</v>
@@ -12074,7 +12069,7 @@
         <v>147</v>
       </c>
       <c r="E11" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="F11">
         <v>0.99</v>
@@ -12173,7 +12168,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>243</v>
@@ -12184,7 +12179,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>244</v>
@@ -12195,7 +12190,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>245</v>
@@ -12206,7 +12201,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>144</v>
@@ -12217,7 +12212,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>145</v>
@@ -12228,7 +12223,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>243</v>
@@ -12239,7 +12234,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>244</v>
@@ -12250,7 +12245,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>245</v>
@@ -12261,7 +12256,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>144</v>
@@ -12272,7 +12267,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>145</v>
@@ -12283,24 +12278,24 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>333</v>
+      </c>
+      <c r="B12" t="s">
         <v>334</v>
       </c>
-      <c r="B12" t="s">
-        <v>336</v>
-      </c>
       <c r="C12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B13" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C13" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -12372,7 +12367,7 @@
         <v>247</v>
       </c>
       <c r="B5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C5" t="s">
         <v>248</v>
@@ -12383,7 +12378,7 @@
         <v>247</v>
       </c>
       <c r="B6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C6" t="s">
         <v>248</v>
@@ -12394,7 +12389,7 @@
         <v>247</v>
       </c>
       <c r="B7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C7" t="s">
         <v>248</v>
@@ -12405,7 +12400,7 @@
         <v>247</v>
       </c>
       <c r="B8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C8" t="s">
         <v>248</v>
@@ -12416,7 +12411,7 @@
         <v>247</v>
       </c>
       <c r="B9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C9" t="s">
         <v>248</v>
@@ -12427,7 +12422,7 @@
         <v>247</v>
       </c>
       <c r="B10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C10" t="s">
         <v>248</v>
@@ -12438,7 +12433,7 @@
         <v>247</v>
       </c>
       <c r="B11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C11" t="s">
         <v>248</v>
@@ -12449,7 +12444,7 @@
         <v>247</v>
       </c>
       <c r="B12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C12" t="s">
         <v>248</v>
@@ -12460,7 +12455,7 @@
         <v>247</v>
       </c>
       <c r="B13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C13" t="s">
         <v>248</v>
@@ -12471,7 +12466,7 @@
         <v>247</v>
       </c>
       <c r="B14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C14" t="s">
         <v>248</v>
@@ -12482,7 +12477,7 @@
         <v>247</v>
       </c>
       <c r="B15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C15" t="s">
         <v>248</v>
@@ -12493,7 +12488,7 @@
         <v>247</v>
       </c>
       <c r="B16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C16" t="s">
         <v>248</v>
@@ -12504,7 +12499,7 @@
         <v>247</v>
       </c>
       <c r="B17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C17" t="s">
         <v>248</v>
@@ -12515,7 +12510,7 @@
         <v>247</v>
       </c>
       <c r="B18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C18" t="s">
         <v>248</v>
@@ -12526,7 +12521,7 @@
         <v>247</v>
       </c>
       <c r="B19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C19" t="s">
         <v>248</v>
@@ -12537,7 +12532,7 @@
         <v>247</v>
       </c>
       <c r="B20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C20" t="s">
         <v>248</v>
@@ -12548,7 +12543,7 @@
         <v>247</v>
       </c>
       <c r="B21" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C21" t="s">
         <v>248</v>
@@ -12559,7 +12554,7 @@
         <v>247</v>
       </c>
       <c r="B22" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C22" t="s">
         <v>248</v>
@@ -12570,7 +12565,7 @@
         <v>247</v>
       </c>
       <c r="B23" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C23" t="s">
         <v>248</v>
@@ -12581,7 +12576,7 @@
         <v>247</v>
       </c>
       <c r="B24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C24" t="s">
         <v>248</v>
@@ -12592,7 +12587,7 @@
         <v>247</v>
       </c>
       <c r="B25" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C25" t="s">
         <v>248</v>
@@ -12603,7 +12598,7 @@
         <v>247</v>
       </c>
       <c r="B26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C26" t="s">
         <v>248</v>
@@ -12614,7 +12609,7 @@
         <v>247</v>
       </c>
       <c r="B27" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C27" t="s">
         <v>248</v>
@@ -12625,7 +12620,7 @@
         <v>247</v>
       </c>
       <c r="B28" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C28" t="s">
         <v>248</v>
@@ -12636,7 +12631,7 @@
         <v>247</v>
       </c>
       <c r="B29" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C29" t="s">
         <v>248</v>
@@ -12647,7 +12642,7 @@
         <v>247</v>
       </c>
       <c r="B30" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C30" t="s">
         <v>248</v>
@@ -12658,7 +12653,7 @@
         <v>247</v>
       </c>
       <c r="B31" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C31" t="s">
         <v>248</v>
@@ -12669,7 +12664,7 @@
         <v>247</v>
       </c>
       <c r="B32" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C32" t="s">
         <v>248</v>
@@ -12680,7 +12675,7 @@
         <v>247</v>
       </c>
       <c r="B33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C33" t="s">
         <v>248</v>
@@ -12691,7 +12686,7 @@
         <v>247</v>
       </c>
       <c r="B34" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C34" t="s">
         <v>248</v>
@@ -12702,7 +12697,7 @@
         <v>247</v>
       </c>
       <c r="B35" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C35" t="s">
         <v>248</v>
@@ -12713,7 +12708,7 @@
         <v>247</v>
       </c>
       <c r="B36" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C36" t="s">
         <v>248</v>
@@ -12724,7 +12719,7 @@
         <v>247</v>
       </c>
       <c r="B37" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C37" t="s">
         <v>248</v>
@@ -12735,7 +12730,7 @@
         <v>247</v>
       </c>
       <c r="B38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C38" t="s">
         <v>248</v>
@@ -12746,7 +12741,7 @@
         <v>247</v>
       </c>
       <c r="B39" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C39" t="s">
         <v>248</v>
@@ -12757,7 +12752,7 @@
         <v>247</v>
       </c>
       <c r="B40" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C40" t="s">
         <v>248</v>
@@ -12768,7 +12763,7 @@
         <v>247</v>
       </c>
       <c r="B41" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C41" t="s">
         <v>248</v>
@@ -12779,7 +12774,7 @@
         <v>247</v>
       </c>
       <c r="B42" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C42" t="s">
         <v>248</v>
@@ -12790,7 +12785,7 @@
         <v>247</v>
       </c>
       <c r="B43" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C43" t="s">
         <v>248</v>
@@ -12801,7 +12796,7 @@
         <v>247</v>
       </c>
       <c r="B44" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C44" t="s">
         <v>248</v>
@@ -12812,7 +12807,7 @@
         <v>247</v>
       </c>
       <c r="B45" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C45" t="s">
         <v>248</v>
@@ -12823,7 +12818,7 @@
         <v>247</v>
       </c>
       <c r="B46" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C46" t="s">
         <v>248</v>
@@ -12834,7 +12829,7 @@
         <v>247</v>
       </c>
       <c r="B47" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C47" t="s">
         <v>248</v>
@@ -12845,7 +12840,7 @@
         <v>247</v>
       </c>
       <c r="B48" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C48" t="s">
         <v>248</v>
@@ -12856,7 +12851,7 @@
         <v>247</v>
       </c>
       <c r="B49" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C49" t="s">
         <v>248</v>
@@ -12867,7 +12862,7 @@
         <v>247</v>
       </c>
       <c r="B50" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C50" t="s">
         <v>248</v>
@@ -12878,7 +12873,7 @@
         <v>247</v>
       </c>
       <c r="B51" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C51" t="s">
         <v>248</v>
@@ -12889,7 +12884,7 @@
         <v>247</v>
       </c>
       <c r="B52" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C52" t="s">
         <v>248</v>
@@ -12900,7 +12895,7 @@
         <v>247</v>
       </c>
       <c r="B53" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C53" t="s">
         <v>248</v>
@@ -12911,7 +12906,7 @@
         <v>247</v>
       </c>
       <c r="B54" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C54" t="s">
         <v>248</v>
@@ -12922,7 +12917,7 @@
         <v>247</v>
       </c>
       <c r="B55" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C55" t="s">
         <v>248</v>
@@ -12933,7 +12928,7 @@
         <v>247</v>
       </c>
       <c r="B56" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C56" t="s">
         <v>248</v>
@@ -12944,7 +12939,7 @@
         <v>247</v>
       </c>
       <c r="B57" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C57" t="s">
         <v>248</v>
@@ -12955,7 +12950,7 @@
         <v>247</v>
       </c>
       <c r="B58" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C58" t="s">
         <v>248</v>
@@ -12966,7 +12961,7 @@
         <v>247</v>
       </c>
       <c r="B59" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C59" t="s">
         <v>248</v>
@@ -12977,7 +12972,7 @@
         <v>247</v>
       </c>
       <c r="B60" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C60" t="s">
         <v>248</v>
@@ -12988,7 +12983,7 @@
         <v>247</v>
       </c>
       <c r="B61" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C61" t="s">
         <v>248</v>
@@ -12999,7 +12994,7 @@
         <v>247</v>
       </c>
       <c r="B62" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C62" t="s">
         <v>248</v>
@@ -13010,7 +13005,7 @@
         <v>247</v>
       </c>
       <c r="B63" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C63" t="s">
         <v>248</v>
@@ -13021,7 +13016,7 @@
         <v>247</v>
       </c>
       <c r="B64" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C64" t="s">
         <v>248</v>
@@ -13032,7 +13027,7 @@
         <v>247</v>
       </c>
       <c r="B65" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C65" t="s">
         <v>248</v>
@@ -13043,7 +13038,7 @@
         <v>247</v>
       </c>
       <c r="B66" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C66" t="s">
         <v>248</v>
@@ -13054,7 +13049,7 @@
         <v>247</v>
       </c>
       <c r="B67" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C67" t="s">
         <v>248</v>
@@ -13065,7 +13060,7 @@
         <v>247</v>
       </c>
       <c r="B68" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C68" t="s">
         <v>248</v>
@@ -13076,7 +13071,7 @@
         <v>247</v>
       </c>
       <c r="B69" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C69" t="s">
         <v>248</v>
@@ -13087,7 +13082,7 @@
         <v>247</v>
       </c>
       <c r="B70" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C70" t="s">
         <v>248</v>
@@ -13098,7 +13093,7 @@
         <v>247</v>
       </c>
       <c r="B71" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C71" t="s">
         <v>248</v>
@@ -13109,7 +13104,7 @@
         <v>247</v>
       </c>
       <c r="B72" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C72" t="s">
         <v>248</v>
@@ -13120,7 +13115,7 @@
         <v>247</v>
       </c>
       <c r="B73" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C73" t="s">
         <v>248</v>
@@ -13131,7 +13126,7 @@
         <v>247</v>
       </c>
       <c r="B74" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C74" t="s">
         <v>248</v>
@@ -13142,7 +13137,7 @@
         <v>247</v>
       </c>
       <c r="B75" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C75" t="s">
         <v>248</v>
@@ -13153,7 +13148,7 @@
         <v>247</v>
       </c>
       <c r="B76" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C76" t="s">
         <v>248</v>
@@ -13164,7 +13159,7 @@
         <v>247</v>
       </c>
       <c r="B77" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C77" t="s">
         <v>248</v>
@@ -13175,7 +13170,7 @@
         <v>247</v>
       </c>
       <c r="B78" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C78" t="s">
         <v>248</v>
@@ -13186,7 +13181,7 @@
         <v>247</v>
       </c>
       <c r="B79" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C79" t="s">
         <v>248</v>
@@ -13197,7 +13192,7 @@
         <v>247</v>
       </c>
       <c r="B80" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C80" t="s">
         <v>248</v>
@@ -13208,7 +13203,7 @@
         <v>247</v>
       </c>
       <c r="B81" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C81" t="s">
         <v>248</v>
@@ -13219,7 +13214,7 @@
         <v>247</v>
       </c>
       <c r="B82" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C82" t="s">
         <v>248</v>
@@ -13230,7 +13225,7 @@
         <v>247</v>
       </c>
       <c r="B83" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C83" t="s">
         <v>248</v>
@@ -13241,7 +13236,7 @@
         <v>247</v>
       </c>
       <c r="B84" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C84" t="s">
         <v>248</v>
@@ -13252,7 +13247,7 @@
         <v>247</v>
       </c>
       <c r="B85" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C85" t="s">
         <v>248</v>
@@ -13263,7 +13258,7 @@
         <v>247</v>
       </c>
       <c r="B86" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C86" t="s">
         <v>248</v>
@@ -13308,7 +13303,7 @@
         <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -13319,7 +13314,7 @@
         <v>147</v>
       </c>
       <c r="C3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -13330,7 +13325,7 @@
         <v>150</v>
       </c>
       <c r="C4" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -13338,10 +13333,10 @@
         <v>250</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -13349,10 +13344,10 @@
         <v>250</v>
       </c>
       <c r="B6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -13360,10 +13355,10 @@
         <v>250</v>
       </c>
       <c r="B7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C7" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -13371,10 +13366,10 @@
         <v>250</v>
       </c>
       <c r="B8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C8" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -13382,10 +13377,10 @@
         <v>250</v>
       </c>
       <c r="B9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C9" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -13393,10 +13388,10 @@
         <v>250</v>
       </c>
       <c r="B10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C10" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -13404,10 +13399,10 @@
         <v>250</v>
       </c>
       <c r="B11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C11" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -13415,10 +13410,10 @@
         <v>250</v>
       </c>
       <c r="B12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C12" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -13426,10 +13421,10 @@
         <v>250</v>
       </c>
       <c r="B13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C13" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -13437,10 +13432,10 @@
         <v>250</v>
       </c>
       <c r="B14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C14" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -13448,10 +13443,10 @@
         <v>250</v>
       </c>
       <c r="B15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C15" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -13459,10 +13454,10 @@
         <v>250</v>
       </c>
       <c r="B16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C16" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -13470,10 +13465,10 @@
         <v>250</v>
       </c>
       <c r="B17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C17" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -13481,10 +13476,10 @@
         <v>250</v>
       </c>
       <c r="B18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C18" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -13492,10 +13487,10 @@
         <v>250</v>
       </c>
       <c r="B19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -13503,10 +13498,10 @@
         <v>250</v>
       </c>
       <c r="B20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C20" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -13514,10 +13509,10 @@
         <v>250</v>
       </c>
       <c r="B21" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C21" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -13525,10 +13520,10 @@
         <v>250</v>
       </c>
       <c r="B22" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C22" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -13536,10 +13531,10 @@
         <v>250</v>
       </c>
       <c r="B23" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C23" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -13547,10 +13542,10 @@
         <v>250</v>
       </c>
       <c r="B24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C24" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -13558,10 +13553,10 @@
         <v>250</v>
       </c>
       <c r="B25" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C25" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -13569,10 +13564,10 @@
         <v>250</v>
       </c>
       <c r="B26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C26" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -13580,10 +13575,10 @@
         <v>250</v>
       </c>
       <c r="B27" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C27" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -13591,10 +13586,10 @@
         <v>250</v>
       </c>
       <c r="B28" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C28" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -13602,10 +13597,10 @@
         <v>250</v>
       </c>
       <c r="B29" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C29" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -13613,10 +13608,10 @@
         <v>250</v>
       </c>
       <c r="B30" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C30" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -13624,10 +13619,10 @@
         <v>250</v>
       </c>
       <c r="B31" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C31" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -13635,10 +13630,10 @@
         <v>250</v>
       </c>
       <c r="B32" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C32" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -13646,10 +13641,10 @@
         <v>250</v>
       </c>
       <c r="B33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C33" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -13657,10 +13652,10 @@
         <v>250</v>
       </c>
       <c r="B34" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C34" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -13668,10 +13663,10 @@
         <v>250</v>
       </c>
       <c r="B35" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C35" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -13679,10 +13674,10 @@
         <v>250</v>
       </c>
       <c r="B36" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C36" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -13690,10 +13685,10 @@
         <v>250</v>
       </c>
       <c r="B37" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C37" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -13701,10 +13696,10 @@
         <v>250</v>
       </c>
       <c r="B38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C38" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -13712,10 +13707,10 @@
         <v>250</v>
       </c>
       <c r="B39" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C39" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
@@ -13723,10 +13718,10 @@
         <v>250</v>
       </c>
       <c r="B40" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C40" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
@@ -13734,10 +13729,10 @@
         <v>250</v>
       </c>
       <c r="B41" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C41" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -13745,10 +13740,10 @@
         <v>250</v>
       </c>
       <c r="B42" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C42" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
@@ -13756,10 +13751,10 @@
         <v>250</v>
       </c>
       <c r="B43" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C43" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -13767,10 +13762,10 @@
         <v>250</v>
       </c>
       <c r="B44" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C44" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -13778,10 +13773,10 @@
         <v>250</v>
       </c>
       <c r="B45" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C45" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
@@ -13789,10 +13784,10 @@
         <v>250</v>
       </c>
       <c r="B46" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C46" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
@@ -13800,10 +13795,10 @@
         <v>250</v>
       </c>
       <c r="B47" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C47" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
@@ -13811,10 +13806,10 @@
         <v>250</v>
       </c>
       <c r="B48" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C48" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -13822,10 +13817,10 @@
         <v>250</v>
       </c>
       <c r="B49" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C49" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -13833,10 +13828,10 @@
         <v>250</v>
       </c>
       <c r="B50" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C50" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -13844,10 +13839,10 @@
         <v>250</v>
       </c>
       <c r="B51" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C51" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -13855,10 +13850,10 @@
         <v>250</v>
       </c>
       <c r="B52" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C52" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
@@ -13866,10 +13861,10 @@
         <v>250</v>
       </c>
       <c r="B53" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C53" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
@@ -13877,10 +13872,10 @@
         <v>250</v>
       </c>
       <c r="B54" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C54" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -13888,10 +13883,10 @@
         <v>250</v>
       </c>
       <c r="B55" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C55" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
@@ -13899,10 +13894,10 @@
         <v>250</v>
       </c>
       <c r="B56" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C56" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
@@ -13910,10 +13905,10 @@
         <v>250</v>
       </c>
       <c r="B57" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C57" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
@@ -13921,10 +13916,10 @@
         <v>250</v>
       </c>
       <c r="B58" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C58" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
@@ -13932,10 +13927,10 @@
         <v>250</v>
       </c>
       <c r="B59" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C59" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
@@ -13943,10 +13938,10 @@
         <v>250</v>
       </c>
       <c r="B60" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C60" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
@@ -13954,10 +13949,10 @@
         <v>250</v>
       </c>
       <c r="B61" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C61" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
@@ -13965,10 +13960,10 @@
         <v>250</v>
       </c>
       <c r="B62" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C62" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
@@ -13976,10 +13971,10 @@
         <v>250</v>
       </c>
       <c r="B63" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C63" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
@@ -13987,10 +13982,10 @@
         <v>250</v>
       </c>
       <c r="B64" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C64" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
@@ -13998,10 +13993,10 @@
         <v>250</v>
       </c>
       <c r="B65" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C65" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
@@ -14009,10 +14004,10 @@
         <v>250</v>
       </c>
       <c r="B66" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C66" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
@@ -14020,10 +14015,10 @@
         <v>250</v>
       </c>
       <c r="B67" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C67" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
@@ -14031,10 +14026,10 @@
         <v>250</v>
       </c>
       <c r="B68" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C68" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
@@ -14042,10 +14037,10 @@
         <v>250</v>
       </c>
       <c r="B69" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C69" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
@@ -14053,10 +14048,10 @@
         <v>250</v>
       </c>
       <c r="B70" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C70" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
@@ -14064,10 +14059,10 @@
         <v>250</v>
       </c>
       <c r="B71" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C71" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
@@ -14075,10 +14070,10 @@
         <v>250</v>
       </c>
       <c r="B72" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C72" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
@@ -14086,10 +14081,10 @@
         <v>250</v>
       </c>
       <c r="B73" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C73" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
@@ -14097,10 +14092,10 @@
         <v>250</v>
       </c>
       <c r="B74" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C74" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
@@ -14108,10 +14103,10 @@
         <v>250</v>
       </c>
       <c r="B75" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C75" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
@@ -14119,10 +14114,10 @@
         <v>250</v>
       </c>
       <c r="B76" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C76" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
@@ -14130,10 +14125,10 @@
         <v>250</v>
       </c>
       <c r="B77" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C77" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
@@ -14141,10 +14136,10 @@
         <v>250</v>
       </c>
       <c r="B78" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C78" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
@@ -14152,10 +14147,10 @@
         <v>250</v>
       </c>
       <c r="B79" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C79" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
@@ -14163,10 +14158,10 @@
         <v>250</v>
       </c>
       <c r="B80" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C80" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
@@ -14174,10 +14169,10 @@
         <v>250</v>
       </c>
       <c r="B81" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C81" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
@@ -14185,10 +14180,10 @@
         <v>250</v>
       </c>
       <c r="B82" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C82" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
@@ -14196,10 +14191,10 @@
         <v>250</v>
       </c>
       <c r="B83" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C83" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
@@ -14207,10 +14202,10 @@
         <v>250</v>
       </c>
       <c r="B84" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C84" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
@@ -14218,10 +14213,10 @@
         <v>250</v>
       </c>
       <c r="B85" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C85" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
@@ -14229,10 +14224,10 @@
         <v>250</v>
       </c>
       <c r="B86" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C86" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
@@ -14243,7 +14238,7 @@
         <v>146</v>
       </c>
       <c r="C87" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
@@ -14254,7 +14249,7 @@
         <v>147</v>
       </c>
       <c r="C88" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
@@ -14265,7 +14260,7 @@
         <v>150</v>
       </c>
       <c r="C89" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
@@ -14273,10 +14268,10 @@
         <v>250</v>
       </c>
       <c r="B90" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C90" s="3" t="s">
         <v>338</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
@@ -14284,10 +14279,10 @@
         <v>250</v>
       </c>
       <c r="B91" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C91" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
@@ -14295,10 +14290,10 @@
         <v>250</v>
       </c>
       <c r="B92" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C92" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
@@ -14306,10 +14301,10 @@
         <v>250</v>
       </c>
       <c r="B93" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C93" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
@@ -14317,10 +14312,10 @@
         <v>250</v>
       </c>
       <c r="B94" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C94" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
@@ -14328,10 +14323,10 @@
         <v>250</v>
       </c>
       <c r="B95" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C95" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
@@ -14339,10 +14334,10 @@
         <v>250</v>
       </c>
       <c r="B96" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C96" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
@@ -14350,10 +14345,10 @@
         <v>250</v>
       </c>
       <c r="B97" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C97" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
@@ -14361,10 +14356,10 @@
         <v>250</v>
       </c>
       <c r="B98" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C98" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
@@ -14372,10 +14367,10 @@
         <v>250</v>
       </c>
       <c r="B99" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C99" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
@@ -14383,10 +14378,10 @@
         <v>250</v>
       </c>
       <c r="B100" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C100" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
@@ -14394,10 +14389,10 @@
         <v>250</v>
       </c>
       <c r="B101" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C101" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
@@ -14405,10 +14400,10 @@
         <v>250</v>
       </c>
       <c r="B102" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C102" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
@@ -14416,10 +14411,10 @@
         <v>250</v>
       </c>
       <c r="B103" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C103" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
@@ -14427,10 +14422,10 @@
         <v>250</v>
       </c>
       <c r="B104" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C104" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
@@ -14438,10 +14433,10 @@
         <v>250</v>
       </c>
       <c r="B105" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C105" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
@@ -14449,10 +14444,10 @@
         <v>250</v>
       </c>
       <c r="B106" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C106" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
@@ -14460,10 +14455,10 @@
         <v>250</v>
       </c>
       <c r="B107" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C107" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
@@ -14471,10 +14466,10 @@
         <v>250</v>
       </c>
       <c r="B108" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C108" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
@@ -14482,10 +14477,10 @@
         <v>250</v>
       </c>
       <c r="B109" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C109" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
@@ -14493,10 +14488,10 @@
         <v>250</v>
       </c>
       <c r="B110" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C110" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
@@ -14504,10 +14499,10 @@
         <v>250</v>
       </c>
       <c r="B111" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C111" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
@@ -14515,10 +14510,10 @@
         <v>250</v>
       </c>
       <c r="B112" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C112" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
@@ -14526,10 +14521,10 @@
         <v>250</v>
       </c>
       <c r="B113" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C113" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
@@ -14537,10 +14532,10 @@
         <v>250</v>
       </c>
       <c r="B114" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C114" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
@@ -14548,10 +14543,10 @@
         <v>250</v>
       </c>
       <c r="B115" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C115" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
@@ -14559,10 +14554,10 @@
         <v>250</v>
       </c>
       <c r="B116" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C116" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
@@ -14570,10 +14565,10 @@
         <v>250</v>
       </c>
       <c r="B117" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C117" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
@@ -14581,10 +14576,10 @@
         <v>250</v>
       </c>
       <c r="B118" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C118" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
@@ -14592,10 +14587,10 @@
         <v>250</v>
       </c>
       <c r="B119" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C119" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
@@ -14603,10 +14598,10 @@
         <v>250</v>
       </c>
       <c r="B120" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C120" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
@@ -14614,10 +14609,10 @@
         <v>250</v>
       </c>
       <c r="B121" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C121" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
@@ -14625,10 +14620,10 @@
         <v>250</v>
       </c>
       <c r="B122" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C122" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
@@ -14636,10 +14631,10 @@
         <v>250</v>
       </c>
       <c r="B123" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C123" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
@@ -14647,10 +14642,10 @@
         <v>250</v>
       </c>
       <c r="B124" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C124" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
@@ -14658,10 +14653,10 @@
         <v>250</v>
       </c>
       <c r="B125" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C125" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
@@ -14669,10 +14664,10 @@
         <v>250</v>
       </c>
       <c r="B126" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C126" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
@@ -14680,10 +14675,10 @@
         <v>250</v>
       </c>
       <c r="B127" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C127" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
@@ -14691,10 +14686,10 @@
         <v>250</v>
       </c>
       <c r="B128" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C128" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
@@ -14702,10 +14697,10 @@
         <v>250</v>
       </c>
       <c r="B129" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C129" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
@@ -14713,10 +14708,10 @@
         <v>250</v>
       </c>
       <c r="B130" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C130" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
@@ -14724,10 +14719,10 @@
         <v>250</v>
       </c>
       <c r="B131" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C131" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
@@ -14735,10 +14730,10 @@
         <v>250</v>
       </c>
       <c r="B132" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C132" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
@@ -14746,10 +14741,10 @@
         <v>250</v>
       </c>
       <c r="B133" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C133" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
@@ -14757,10 +14752,10 @@
         <v>250</v>
       </c>
       <c r="B134" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C134" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
@@ -14768,10 +14763,10 @@
         <v>250</v>
       </c>
       <c r="B135" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C135" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
@@ -14779,10 +14774,10 @@
         <v>250</v>
       </c>
       <c r="B136" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C136" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
@@ -14790,10 +14785,10 @@
         <v>250</v>
       </c>
       <c r="B137" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C137" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
@@ -14801,10 +14796,10 @@
         <v>250</v>
       </c>
       <c r="B138" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C138" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
@@ -14812,10 +14807,10 @@
         <v>250</v>
       </c>
       <c r="B139" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C139" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
@@ -14823,10 +14818,10 @@
         <v>250</v>
       </c>
       <c r="B140" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C140" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
@@ -14834,10 +14829,10 @@
         <v>250</v>
       </c>
       <c r="B141" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C141" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
@@ -14845,10 +14840,10 @@
         <v>250</v>
       </c>
       <c r="B142" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C142" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
@@ -14856,10 +14851,10 @@
         <v>250</v>
       </c>
       <c r="B143" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C143" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
@@ -14867,10 +14862,10 @@
         <v>250</v>
       </c>
       <c r="B144" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C144" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
@@ -14878,10 +14873,10 @@
         <v>250</v>
       </c>
       <c r="B145" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C145" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
@@ -14889,10 +14884,10 @@
         <v>250</v>
       </c>
       <c r="B146" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C146" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
@@ -14900,10 +14895,10 @@
         <v>250</v>
       </c>
       <c r="B147" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C147" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
@@ -14911,10 +14906,10 @@
         <v>250</v>
       </c>
       <c r="B148" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C148" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
@@ -14922,10 +14917,10 @@
         <v>250</v>
       </c>
       <c r="B149" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C149" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
@@ -14933,10 +14928,10 @@
         <v>250</v>
       </c>
       <c r="B150" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C150" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
@@ -14944,10 +14939,10 @@
         <v>250</v>
       </c>
       <c r="B151" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C151" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
@@ -14955,10 +14950,10 @@
         <v>250</v>
       </c>
       <c r="B152" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C152" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
@@ -14966,10 +14961,10 @@
         <v>250</v>
       </c>
       <c r="B153" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C153" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
@@ -14977,10 +14972,10 @@
         <v>250</v>
       </c>
       <c r="B154" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C154" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
@@ -14988,10 +14983,10 @@
         <v>250</v>
       </c>
       <c r="B155" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C155" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
@@ -14999,10 +14994,10 @@
         <v>250</v>
       </c>
       <c r="B156" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C156" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
@@ -15010,10 +15005,10 @@
         <v>250</v>
       </c>
       <c r="B157" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C157" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
@@ -15021,10 +15016,10 @@
         <v>250</v>
       </c>
       <c r="B158" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C158" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
@@ -15032,10 +15027,10 @@
         <v>250</v>
       </c>
       <c r="B159" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C159" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
@@ -15043,10 +15038,10 @@
         <v>250</v>
       </c>
       <c r="B160" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C160" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
@@ -15054,10 +15049,10 @@
         <v>250</v>
       </c>
       <c r="B161" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C161" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
@@ -15065,10 +15060,10 @@
         <v>250</v>
       </c>
       <c r="B162" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C162" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
@@ -15076,10 +15071,10 @@
         <v>250</v>
       </c>
       <c r="B163" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C163" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
@@ -15087,10 +15082,10 @@
         <v>250</v>
       </c>
       <c r="B164" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C164" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
@@ -15098,10 +15093,10 @@
         <v>250</v>
       </c>
       <c r="B165" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C165" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
@@ -15109,10 +15104,10 @@
         <v>250</v>
       </c>
       <c r="B166" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C166" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
@@ -15120,10 +15115,10 @@
         <v>250</v>
       </c>
       <c r="B167" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C167" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
@@ -15131,10 +15126,10 @@
         <v>250</v>
       </c>
       <c r="B168" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C168" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
@@ -15142,10 +15137,10 @@
         <v>250</v>
       </c>
       <c r="B169" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C169" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
@@ -15153,10 +15148,10 @@
         <v>250</v>
       </c>
       <c r="B170" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C170" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
@@ -15164,10 +15159,10 @@
         <v>250</v>
       </c>
       <c r="B171" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C171" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update system model settings
</commit_message>
<xml_diff>
--- a/spine_rts-gmlc/datasets/branch.xlsx
+++ b/spine_rts-gmlc/datasets/branch.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="branch" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="338">
   <si>
     <t>UID</t>
   </si>
@@ -1028,15 +1028,6 @@
   </si>
   <si>
     <t>connection__node</t>
-  </si>
-  <si>
-    <t>in_stor</t>
-  </si>
-  <si>
-    <t>out_stor</t>
-  </si>
-  <si>
-    <t>RES_gen-212_CSP_1_out</t>
   </si>
   <si>
     <t>blk_t1</t>
@@ -11197,10 +11188,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A7" sqref="A7:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11259,22 +11250,6 @@
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B7" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>135</v>
-      </c>
-      <c r="B8" t="s">
-        <v>335</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11282,10 +11257,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11337,7 +11312,7 @@
         <v>148</v>
       </c>
       <c r="E2" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F2">
         <v>175</v>
@@ -11357,7 +11332,7 @@
         <v>149</v>
       </c>
       <c r="E3" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F3">
         <v>175</v>
@@ -11377,7 +11352,7 @@
         <v>148</v>
       </c>
       <c r="E4" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F4">
         <v>175</v>
@@ -11397,7 +11372,7 @@
         <v>149</v>
       </c>
       <c r="E5" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F5">
         <v>175</v>
@@ -11417,7 +11392,7 @@
         <v>148</v>
       </c>
       <c r="E6" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F6">
         <v>500</v>
@@ -11437,7 +11412,7 @@
         <v>149</v>
       </c>
       <c r="E7" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F7">
         <v>500</v>
@@ -11457,7 +11432,7 @@
         <v>148</v>
       </c>
       <c r="E8" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F8">
         <v>500</v>
@@ -11477,7 +11452,7 @@
         <v>149</v>
       </c>
       <c r="E9" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F9">
         <v>500</v>
@@ -11497,7 +11472,7 @@
         <v>148</v>
       </c>
       <c r="E10" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F10">
         <v>500</v>
@@ -11517,7 +11492,7 @@
         <v>149</v>
       </c>
       <c r="E11" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F11">
         <v>500</v>
@@ -11537,7 +11512,7 @@
         <v>148</v>
       </c>
       <c r="E12" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F12">
         <v>500</v>
@@ -11557,7 +11532,7 @@
         <v>149</v>
       </c>
       <c r="E13" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F13">
         <v>500</v>
@@ -11577,7 +11552,7 @@
         <v>148</v>
       </c>
       <c r="E14" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F14">
         <v>500</v>
@@ -11597,7 +11572,7 @@
         <v>149</v>
       </c>
       <c r="E15" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F15">
         <v>500</v>
@@ -11617,7 +11592,7 @@
         <v>148</v>
       </c>
       <c r="E16" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F16">
         <v>500</v>
@@ -11637,7 +11612,7 @@
         <v>149</v>
       </c>
       <c r="E17" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F17">
         <v>500</v>
@@ -11657,7 +11632,7 @@
         <v>148</v>
       </c>
       <c r="E18" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F18">
         <v>500</v>
@@ -11677,7 +11652,7 @@
         <v>149</v>
       </c>
       <c r="E19" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F19">
         <v>500</v>
@@ -11697,7 +11672,7 @@
         <v>148</v>
       </c>
       <c r="E20" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F20">
         <v>500</v>
@@ -11717,42 +11692,22 @@
         <v>149</v>
       </c>
       <c r="E21" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F21">
         <v>500</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>140</v>
-      </c>
-      <c r="B22" t="s">
-        <v>334</v>
-      </c>
-      <c r="C22" t="s">
-        <v>251</v>
-      </c>
-      <c r="D22" t="s">
-        <v>148</v>
-      </c>
+      <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>140</v>
-      </c>
-      <c r="B23" t="s">
-        <v>335</v>
-      </c>
-      <c r="C23" t="s">
-        <v>336</v>
-      </c>
-      <c r="D23" t="s">
-        <v>149</v>
-      </c>
+      <c r="B23" s="1"/>
+      <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B24" s="2"/>
+      <c r="B24" s="1"/>
+      <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
@@ -11795,12 +11750,12 @@
       <c r="I34" s="1"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B35" s="1"/>
-      <c r="I35" s="1"/>
+      <c r="B35" s="2"/>
+      <c r="I35" s="2"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B36" s="1"/>
-      <c r="I36" s="1"/>
+      <c r="B36" s="2"/>
+      <c r="I36" s="2"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B37" s="2"/>
@@ -11825,14 +11780,6 @@
     <row r="42" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B42" s="2"/>
       <c r="I42" s="2"/>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B43" s="2"/>
-      <c r="I43" s="2"/>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B44" s="2"/>
-      <c r="I44" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11844,7 +11791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -11889,7 +11836,7 @@
         <v>147</v>
       </c>
       <c r="E2" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F2">
         <v>0.99</v>
@@ -11909,7 +11856,7 @@
         <v>147</v>
       </c>
       <c r="E3" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F3">
         <v>0.99</v>
@@ -11929,7 +11876,7 @@
         <v>147</v>
       </c>
       <c r="E4" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F4">
         <v>0.99</v>
@@ -11949,7 +11896,7 @@
         <v>150</v>
       </c>
       <c r="E5" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F5">
         <v>0.99</v>
@@ -11969,7 +11916,7 @@
         <v>150</v>
       </c>
       <c r="E6" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F6">
         <v>0.99</v>
@@ -11989,7 +11936,7 @@
         <v>146</v>
       </c>
       <c r="E7" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F7">
         <v>0.99</v>
@@ -12009,7 +11956,7 @@
         <v>146</v>
       </c>
       <c r="E8" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F8">
         <v>0.99</v>
@@ -12029,7 +11976,7 @@
         <v>146</v>
       </c>
       <c r="E9" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F9">
         <v>0.99</v>
@@ -12049,7 +11996,7 @@
         <v>146</v>
       </c>
       <c r="E10" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F10">
         <v>0.99</v>
@@ -12069,7 +12016,7 @@
         <v>147</v>
       </c>
       <c r="E11" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F11">
         <v>0.99</v>
@@ -12142,10 +12089,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12276,28 +12223,6 @@
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>333</v>
-      </c>
-      <c r="B12" t="s">
-        <v>334</v>
-      </c>
-      <c r="C12" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>333</v>
-      </c>
-      <c r="B13" t="s">
-        <v>335</v>
-      </c>
-      <c r="C13" t="s">
-        <v>336</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12305,10 +12230,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C86"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12367,7 +12292,7 @@
         <v>247</v>
       </c>
       <c r="B5" t="s">
-        <v>336</v>
+        <v>251</v>
       </c>
       <c r="C5" t="s">
         <v>248</v>
@@ -12378,7 +12303,7 @@
         <v>247</v>
       </c>
       <c r="B6" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C6" t="s">
         <v>248</v>
@@ -12389,7 +12314,7 @@
         <v>247</v>
       </c>
       <c r="B7" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C7" t="s">
         <v>248</v>
@@ -12400,7 +12325,7 @@
         <v>247</v>
       </c>
       <c r="B8" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C8" t="s">
         <v>248</v>
@@ -12411,7 +12336,7 @@
         <v>247</v>
       </c>
       <c r="B9" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C9" t="s">
         <v>248</v>
@@ -12422,7 +12347,7 @@
         <v>247</v>
       </c>
       <c r="B10" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C10" t="s">
         <v>248</v>
@@ -12433,7 +12358,7 @@
         <v>247</v>
       </c>
       <c r="B11" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C11" t="s">
         <v>248</v>
@@ -12444,7 +12369,7 @@
         <v>247</v>
       </c>
       <c r="B12" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C12" t="s">
         <v>248</v>
@@ -12455,7 +12380,7 @@
         <v>247</v>
       </c>
       <c r="B13" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C13" t="s">
         <v>248</v>
@@ -12466,7 +12391,7 @@
         <v>247</v>
       </c>
       <c r="B14" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C14" t="s">
         <v>248</v>
@@ -12477,7 +12402,7 @@
         <v>247</v>
       </c>
       <c r="B15" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C15" t="s">
         <v>248</v>
@@ -12488,7 +12413,7 @@
         <v>247</v>
       </c>
       <c r="B16" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C16" t="s">
         <v>248</v>
@@ -12499,7 +12424,7 @@
         <v>247</v>
       </c>
       <c r="B17" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C17" t="s">
         <v>248</v>
@@ -12510,7 +12435,7 @@
         <v>247</v>
       </c>
       <c r="B18" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C18" t="s">
         <v>248</v>
@@ -12521,7 +12446,7 @@
         <v>247</v>
       </c>
       <c r="B19" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C19" t="s">
         <v>248</v>
@@ -12532,7 +12457,7 @@
         <v>247</v>
       </c>
       <c r="B20" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C20" t="s">
         <v>248</v>
@@ -12543,7 +12468,7 @@
         <v>247</v>
       </c>
       <c r="B21" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C21" t="s">
         <v>248</v>
@@ -12554,7 +12479,7 @@
         <v>247</v>
       </c>
       <c r="B22" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C22" t="s">
         <v>248</v>
@@ -12565,7 +12490,7 @@
         <v>247</v>
       </c>
       <c r="B23" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C23" t="s">
         <v>248</v>
@@ -12576,7 +12501,7 @@
         <v>247</v>
       </c>
       <c r="B24" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C24" t="s">
         <v>248</v>
@@ -12587,7 +12512,7 @@
         <v>247</v>
       </c>
       <c r="B25" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C25" t="s">
         <v>248</v>
@@ -12598,7 +12523,7 @@
         <v>247</v>
       </c>
       <c r="B26" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C26" t="s">
         <v>248</v>
@@ -12609,7 +12534,7 @@
         <v>247</v>
       </c>
       <c r="B27" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C27" t="s">
         <v>248</v>
@@ -12620,7 +12545,7 @@
         <v>247</v>
       </c>
       <c r="B28" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C28" t="s">
         <v>248</v>
@@ -12631,7 +12556,7 @@
         <v>247</v>
       </c>
       <c r="B29" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C29" t="s">
         <v>248</v>
@@ -12642,7 +12567,7 @@
         <v>247</v>
       </c>
       <c r="B30" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C30" t="s">
         <v>248</v>
@@ -12653,7 +12578,7 @@
         <v>247</v>
       </c>
       <c r="B31" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C31" t="s">
         <v>248</v>
@@ -12664,7 +12589,7 @@
         <v>247</v>
       </c>
       <c r="B32" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C32" t="s">
         <v>248</v>
@@ -12675,7 +12600,7 @@
         <v>247</v>
       </c>
       <c r="B33" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C33" t="s">
         <v>248</v>
@@ -12686,7 +12611,7 @@
         <v>247</v>
       </c>
       <c r="B34" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C34" t="s">
         <v>248</v>
@@ -12697,7 +12622,7 @@
         <v>247</v>
       </c>
       <c r="B35" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C35" t="s">
         <v>248</v>
@@ -12708,7 +12633,7 @@
         <v>247</v>
       </c>
       <c r="B36" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C36" t="s">
         <v>248</v>
@@ -12719,7 +12644,7 @@
         <v>247</v>
       </c>
       <c r="B37" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C37" t="s">
         <v>248</v>
@@ -12730,7 +12655,7 @@
         <v>247</v>
       </c>
       <c r="B38" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C38" t="s">
         <v>248</v>
@@ -12741,7 +12666,7 @@
         <v>247</v>
       </c>
       <c r="B39" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C39" t="s">
         <v>248</v>
@@ -12752,7 +12677,7 @@
         <v>247</v>
       </c>
       <c r="B40" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C40" t="s">
         <v>248</v>
@@ -12763,7 +12688,7 @@
         <v>247</v>
       </c>
       <c r="B41" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C41" t="s">
         <v>248</v>
@@ -12774,7 +12699,7 @@
         <v>247</v>
       </c>
       <c r="B42" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C42" t="s">
         <v>248</v>
@@ -12785,7 +12710,7 @@
         <v>247</v>
       </c>
       <c r="B43" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C43" t="s">
         <v>248</v>
@@ -12796,7 +12721,7 @@
         <v>247</v>
       </c>
       <c r="B44" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C44" t="s">
         <v>248</v>
@@ -12807,7 +12732,7 @@
         <v>247</v>
       </c>
       <c r="B45" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C45" t="s">
         <v>248</v>
@@ -12818,7 +12743,7 @@
         <v>247</v>
       </c>
       <c r="B46" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C46" t="s">
         <v>248</v>
@@ -12829,7 +12754,7 @@
         <v>247</v>
       </c>
       <c r="B47" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C47" t="s">
         <v>248</v>
@@ -12840,7 +12765,7 @@
         <v>247</v>
       </c>
       <c r="B48" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C48" t="s">
         <v>248</v>
@@ -12851,7 +12776,7 @@
         <v>247</v>
       </c>
       <c r="B49" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C49" t="s">
         <v>248</v>
@@ -12862,7 +12787,7 @@
         <v>247</v>
       </c>
       <c r="B50" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C50" t="s">
         <v>248</v>
@@ -12873,7 +12798,7 @@
         <v>247</v>
       </c>
       <c r="B51" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C51" t="s">
         <v>248</v>
@@ -12884,7 +12809,7 @@
         <v>247</v>
       </c>
       <c r="B52" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C52" t="s">
         <v>248</v>
@@ -12895,7 +12820,7 @@
         <v>247</v>
       </c>
       <c r="B53" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C53" t="s">
         <v>248</v>
@@ -12906,7 +12831,7 @@
         <v>247</v>
       </c>
       <c r="B54" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C54" t="s">
         <v>248</v>
@@ -12917,7 +12842,7 @@
         <v>247</v>
       </c>
       <c r="B55" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C55" t="s">
         <v>248</v>
@@ -12928,7 +12853,7 @@
         <v>247</v>
       </c>
       <c r="B56" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C56" t="s">
         <v>248</v>
@@ -12939,7 +12864,7 @@
         <v>247</v>
       </c>
       <c r="B57" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C57" t="s">
         <v>248</v>
@@ -12950,7 +12875,7 @@
         <v>247</v>
       </c>
       <c r="B58" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C58" t="s">
         <v>248</v>
@@ -12961,7 +12886,7 @@
         <v>247</v>
       </c>
       <c r="B59" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C59" t="s">
         <v>248</v>
@@ -12972,7 +12897,7 @@
         <v>247</v>
       </c>
       <c r="B60" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C60" t="s">
         <v>248</v>
@@ -12983,7 +12908,7 @@
         <v>247</v>
       </c>
       <c r="B61" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C61" t="s">
         <v>248</v>
@@ -12994,7 +12919,7 @@
         <v>247</v>
       </c>
       <c r="B62" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C62" t="s">
         <v>248</v>
@@ -13005,7 +12930,7 @@
         <v>247</v>
       </c>
       <c r="B63" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C63" t="s">
         <v>248</v>
@@ -13016,7 +12941,7 @@
         <v>247</v>
       </c>
       <c r="B64" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C64" t="s">
         <v>248</v>
@@ -13027,7 +12952,7 @@
         <v>247</v>
       </c>
       <c r="B65" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C65" t="s">
         <v>248</v>
@@ -13038,7 +12963,7 @@
         <v>247</v>
       </c>
       <c r="B66" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C66" t="s">
         <v>248</v>
@@ -13049,7 +12974,7 @@
         <v>247</v>
       </c>
       <c r="B67" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C67" t="s">
         <v>248</v>
@@ -13060,7 +12985,7 @@
         <v>247</v>
       </c>
       <c r="B68" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C68" t="s">
         <v>248</v>
@@ -13071,7 +12996,7 @@
         <v>247</v>
       </c>
       <c r="B69" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C69" t="s">
         <v>248</v>
@@ -13082,7 +13007,7 @@
         <v>247</v>
       </c>
       <c r="B70" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C70" t="s">
         <v>248</v>
@@ -13093,7 +13018,7 @@
         <v>247</v>
       </c>
       <c r="B71" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C71" t="s">
         <v>248</v>
@@ -13104,7 +13029,7 @@
         <v>247</v>
       </c>
       <c r="B72" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C72" t="s">
         <v>248</v>
@@ -13115,7 +13040,7 @@
         <v>247</v>
       </c>
       <c r="B73" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C73" t="s">
         <v>248</v>
@@ -13126,7 +13051,7 @@
         <v>247</v>
       </c>
       <c r="B74" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C74" t="s">
         <v>248</v>
@@ -13137,7 +13062,7 @@
         <v>247</v>
       </c>
       <c r="B75" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C75" t="s">
         <v>248</v>
@@ -13148,7 +13073,7 @@
         <v>247</v>
       </c>
       <c r="B76" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C76" t="s">
         <v>248</v>
@@ -13159,7 +13084,7 @@
         <v>247</v>
       </c>
       <c r="B77" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C77" t="s">
         <v>248</v>
@@ -13170,7 +13095,7 @@
         <v>247</v>
       </c>
       <c r="B78" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C78" t="s">
         <v>248</v>
@@ -13181,7 +13106,7 @@
         <v>247</v>
       </c>
       <c r="B79" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C79" t="s">
         <v>248</v>
@@ -13192,7 +13117,7 @@
         <v>247</v>
       </c>
       <c r="B80" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C80" t="s">
         <v>248</v>
@@ -13203,7 +13128,7 @@
         <v>247</v>
       </c>
       <c r="B81" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C81" t="s">
         <v>248</v>
@@ -13214,7 +13139,7 @@
         <v>247</v>
       </c>
       <c r="B82" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C82" t="s">
         <v>248</v>
@@ -13225,7 +13150,7 @@
         <v>247</v>
       </c>
       <c r="B83" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C83" t="s">
         <v>248</v>
@@ -13236,7 +13161,7 @@
         <v>247</v>
       </c>
       <c r="B84" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C84" t="s">
         <v>248</v>
@@ -13247,20 +13172,9 @@
         <v>247</v>
       </c>
       <c r="B85" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C85" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
-        <v>247</v>
-      </c>
-      <c r="B86" t="s">
-        <v>331</v>
-      </c>
-      <c r="C86" t="s">
         <v>248</v>
       </c>
     </row>
@@ -13271,10 +13185,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C171"/>
+  <dimension ref="A1:C169"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="E165" sqref="E165"/>
+    <sheetView topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89:XFD89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13303,7 +13217,7 @@
         <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -13314,7 +13228,7 @@
         <v>147</v>
       </c>
       <c r="C3" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -13325,18 +13239,18 @@
         <v>150</v>
       </c>
       <c r="C4" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>337</v>
+        <v>334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B5" t="s">
+        <v>251</v>
+      </c>
+      <c r="C5" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -13344,10 +13258,10 @@
         <v>250</v>
       </c>
       <c r="B6" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C6" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -13355,10 +13269,10 @@
         <v>250</v>
       </c>
       <c r="B7" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C7" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -13366,10 +13280,10 @@
         <v>250</v>
       </c>
       <c r="B8" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C8" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -13377,10 +13291,10 @@
         <v>250</v>
       </c>
       <c r="B9" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C9" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -13388,10 +13302,10 @@
         <v>250</v>
       </c>
       <c r="B10" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C10" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -13399,10 +13313,10 @@
         <v>250</v>
       </c>
       <c r="B11" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C11" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -13410,10 +13324,10 @@
         <v>250</v>
       </c>
       <c r="B12" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C12" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -13421,10 +13335,10 @@
         <v>250</v>
       </c>
       <c r="B13" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C13" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -13432,10 +13346,10 @@
         <v>250</v>
       </c>
       <c r="B14" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -13443,10 +13357,10 @@
         <v>250</v>
       </c>
       <c r="B15" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C15" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -13454,10 +13368,10 @@
         <v>250</v>
       </c>
       <c r="B16" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C16" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -13465,10 +13379,10 @@
         <v>250</v>
       </c>
       <c r="B17" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C17" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -13476,10 +13390,10 @@
         <v>250</v>
       </c>
       <c r="B18" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C18" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -13487,10 +13401,10 @@
         <v>250</v>
       </c>
       <c r="B19" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C19" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -13498,10 +13412,10 @@
         <v>250</v>
       </c>
       <c r="B20" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C20" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -13509,10 +13423,10 @@
         <v>250</v>
       </c>
       <c r="B21" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -13520,10 +13434,10 @@
         <v>250</v>
       </c>
       <c r="B22" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C22" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -13531,10 +13445,10 @@
         <v>250</v>
       </c>
       <c r="B23" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C23" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -13542,10 +13456,10 @@
         <v>250</v>
       </c>
       <c r="B24" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C24" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -13553,10 +13467,10 @@
         <v>250</v>
       </c>
       <c r="B25" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C25" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -13564,10 +13478,10 @@
         <v>250</v>
       </c>
       <c r="B26" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C26" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -13575,10 +13489,10 @@
         <v>250</v>
       </c>
       <c r="B27" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C27" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -13586,10 +13500,10 @@
         <v>250</v>
       </c>
       <c r="B28" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C28" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -13597,10 +13511,10 @@
         <v>250</v>
       </c>
       <c r="B29" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C29" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -13608,10 +13522,10 @@
         <v>250</v>
       </c>
       <c r="B30" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C30" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -13619,10 +13533,10 @@
         <v>250</v>
       </c>
       <c r="B31" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C31" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -13630,10 +13544,10 @@
         <v>250</v>
       </c>
       <c r="B32" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C32" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -13641,10 +13555,10 @@
         <v>250</v>
       </c>
       <c r="B33" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C33" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -13652,10 +13566,10 @@
         <v>250</v>
       </c>
       <c r="B34" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C34" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -13663,10 +13577,10 @@
         <v>250</v>
       </c>
       <c r="B35" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C35" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -13674,10 +13588,10 @@
         <v>250</v>
       </c>
       <c r="B36" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C36" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -13685,10 +13599,10 @@
         <v>250</v>
       </c>
       <c r="B37" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C37" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -13696,10 +13610,10 @@
         <v>250</v>
       </c>
       <c r="B38" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C38" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -13707,10 +13621,10 @@
         <v>250</v>
       </c>
       <c r="B39" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C39" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
@@ -13718,10 +13632,10 @@
         <v>250</v>
       </c>
       <c r="B40" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C40" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
@@ -13729,10 +13643,10 @@
         <v>250</v>
       </c>
       <c r="B41" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C41" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -13740,10 +13654,10 @@
         <v>250</v>
       </c>
       <c r="B42" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C42" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
@@ -13751,10 +13665,10 @@
         <v>250</v>
       </c>
       <c r="B43" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C43" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -13762,10 +13676,10 @@
         <v>250</v>
       </c>
       <c r="B44" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C44" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -13773,10 +13687,10 @@
         <v>250</v>
       </c>
       <c r="B45" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C45" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
@@ -13784,10 +13698,10 @@
         <v>250</v>
       </c>
       <c r="B46" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C46" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
@@ -13795,10 +13709,10 @@
         <v>250</v>
       </c>
       <c r="B47" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C47" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
@@ -13806,10 +13720,10 @@
         <v>250</v>
       </c>
       <c r="B48" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C48" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -13817,10 +13731,10 @@
         <v>250</v>
       </c>
       <c r="B49" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C49" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -13828,10 +13742,10 @@
         <v>250</v>
       </c>
       <c r="B50" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C50" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -13839,10 +13753,10 @@
         <v>250</v>
       </c>
       <c r="B51" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C51" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -13850,10 +13764,10 @@
         <v>250</v>
       </c>
       <c r="B52" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C52" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
@@ -13861,10 +13775,10 @@
         <v>250</v>
       </c>
       <c r="B53" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C53" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
@@ -13872,10 +13786,10 @@
         <v>250</v>
       </c>
       <c r="B54" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C54" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -13883,10 +13797,10 @@
         <v>250</v>
       </c>
       <c r="B55" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C55" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
@@ -13894,10 +13808,10 @@
         <v>250</v>
       </c>
       <c r="B56" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C56" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
@@ -13905,10 +13819,10 @@
         <v>250</v>
       </c>
       <c r="B57" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C57" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
@@ -13916,10 +13830,10 @@
         <v>250</v>
       </c>
       <c r="B58" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C58" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
@@ -13927,10 +13841,10 @@
         <v>250</v>
       </c>
       <c r="B59" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C59" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
@@ -13938,10 +13852,10 @@
         <v>250</v>
       </c>
       <c r="B60" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C60" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
@@ -13949,10 +13863,10 @@
         <v>250</v>
       </c>
       <c r="B61" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C61" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
@@ -13960,10 +13874,10 @@
         <v>250</v>
       </c>
       <c r="B62" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C62" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
@@ -13971,10 +13885,10 @@
         <v>250</v>
       </c>
       <c r="B63" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C63" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
@@ -13982,10 +13896,10 @@
         <v>250</v>
       </c>
       <c r="B64" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C64" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
@@ -13993,10 +13907,10 @@
         <v>250</v>
       </c>
       <c r="B65" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C65" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
@@ -14004,10 +13918,10 @@
         <v>250</v>
       </c>
       <c r="B66" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C66" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
@@ -14015,10 +13929,10 @@
         <v>250</v>
       </c>
       <c r="B67" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C67" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
@@ -14026,10 +13940,10 @@
         <v>250</v>
       </c>
       <c r="B68" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C68" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
@@ -14037,10 +13951,10 @@
         <v>250</v>
       </c>
       <c r="B69" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C69" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
@@ -14048,10 +13962,10 @@
         <v>250</v>
       </c>
       <c r="B70" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C70" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
@@ -14059,10 +13973,10 @@
         <v>250</v>
       </c>
       <c r="B71" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C71" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
@@ -14070,10 +13984,10 @@
         <v>250</v>
       </c>
       <c r="B72" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C72" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
@@ -14081,10 +13995,10 @@
         <v>250</v>
       </c>
       <c r="B73" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C73" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
@@ -14092,10 +14006,10 @@
         <v>250</v>
       </c>
       <c r="B74" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C74" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
@@ -14103,10 +14017,10 @@
         <v>250</v>
       </c>
       <c r="B75" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C75" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
@@ -14114,10 +14028,10 @@
         <v>250</v>
       </c>
       <c r="B76" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C76" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
@@ -14125,10 +14039,10 @@
         <v>250</v>
       </c>
       <c r="B77" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C77" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
@@ -14136,10 +14050,10 @@
         <v>250</v>
       </c>
       <c r="B78" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C78" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
@@ -14147,10 +14061,10 @@
         <v>250</v>
       </c>
       <c r="B79" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C79" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
@@ -14158,10 +14072,10 @@
         <v>250</v>
       </c>
       <c r="B80" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C80" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
@@ -14169,10 +14083,10 @@
         <v>250</v>
       </c>
       <c r="B81" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C81" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
@@ -14180,10 +14094,10 @@
         <v>250</v>
       </c>
       <c r="B82" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C82" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
@@ -14191,10 +14105,10 @@
         <v>250</v>
       </c>
       <c r="B83" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C83" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
@@ -14202,10 +14116,10 @@
         <v>250</v>
       </c>
       <c r="B84" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C84" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
@@ -14213,10 +14127,10 @@
         <v>250</v>
       </c>
       <c r="B85" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C85" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
@@ -14224,10 +14138,10 @@
         <v>250</v>
       </c>
       <c r="B86" t="s">
-        <v>331</v>
+        <v>146</v>
       </c>
       <c r="C86" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
@@ -14235,10 +14149,10 @@
         <v>250</v>
       </c>
       <c r="B87" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C87" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
@@ -14246,10 +14160,10 @@
         <v>250</v>
       </c>
       <c r="B88" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C88" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
@@ -14257,21 +14171,21 @@
         <v>250</v>
       </c>
       <c r="B89" t="s">
-        <v>150</v>
+        <v>251</v>
       </c>
       <c r="C89" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>338</v>
+      <c r="A90" t="s">
+        <v>250</v>
+      </c>
+      <c r="B90" t="s">
+        <v>252</v>
+      </c>
+      <c r="C90" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
@@ -14279,10 +14193,10 @@
         <v>250</v>
       </c>
       <c r="B91" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C91" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
@@ -14290,10 +14204,10 @@
         <v>250</v>
       </c>
       <c r="B92" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C92" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
@@ -14301,10 +14215,10 @@
         <v>250</v>
       </c>
       <c r="B93" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C93" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
@@ -14312,10 +14226,10 @@
         <v>250</v>
       </c>
       <c r="B94" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C94" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
@@ -14323,10 +14237,10 @@
         <v>250</v>
       </c>
       <c r="B95" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C95" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
@@ -14334,10 +14248,10 @@
         <v>250</v>
       </c>
       <c r="B96" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C96" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
@@ -14345,10 +14259,10 @@
         <v>250</v>
       </c>
       <c r="B97" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C97" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
@@ -14356,10 +14270,10 @@
         <v>250</v>
       </c>
       <c r="B98" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C98" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
@@ -14367,10 +14281,10 @@
         <v>250</v>
       </c>
       <c r="B99" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C99" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
@@ -14378,10 +14292,10 @@
         <v>250</v>
       </c>
       <c r="B100" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C100" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
@@ -14389,10 +14303,10 @@
         <v>250</v>
       </c>
       <c r="B101" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C101" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
@@ -14400,10 +14314,10 @@
         <v>250</v>
       </c>
       <c r="B102" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C102" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
@@ -14411,10 +14325,10 @@
         <v>250</v>
       </c>
       <c r="B103" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C103" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
@@ -14422,10 +14336,10 @@
         <v>250</v>
       </c>
       <c r="B104" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C104" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
@@ -14433,10 +14347,10 @@
         <v>250</v>
       </c>
       <c r="B105" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C105" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
@@ -14444,10 +14358,10 @@
         <v>250</v>
       </c>
       <c r="B106" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C106" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
@@ -14455,10 +14369,10 @@
         <v>250</v>
       </c>
       <c r="B107" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C107" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
@@ -14466,10 +14380,10 @@
         <v>250</v>
       </c>
       <c r="B108" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C108" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
@@ -14477,10 +14391,10 @@
         <v>250</v>
       </c>
       <c r="B109" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C109" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
@@ -14488,10 +14402,10 @@
         <v>250</v>
       </c>
       <c r="B110" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C110" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
@@ -14499,10 +14413,10 @@
         <v>250</v>
       </c>
       <c r="B111" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C111" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
@@ -14510,10 +14424,10 @@
         <v>250</v>
       </c>
       <c r="B112" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C112" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
@@ -14521,10 +14435,10 @@
         <v>250</v>
       </c>
       <c r="B113" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C113" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
@@ -14532,10 +14446,10 @@
         <v>250</v>
       </c>
       <c r="B114" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C114" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
@@ -14543,10 +14457,10 @@
         <v>250</v>
       </c>
       <c r="B115" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C115" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
@@ -14554,10 +14468,10 @@
         <v>250</v>
       </c>
       <c r="B116" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C116" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
@@ -14565,10 +14479,10 @@
         <v>250</v>
       </c>
       <c r="B117" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C117" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
@@ -14576,10 +14490,10 @@
         <v>250</v>
       </c>
       <c r="B118" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C118" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
@@ -14587,10 +14501,10 @@
         <v>250</v>
       </c>
       <c r="B119" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C119" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
@@ -14598,10 +14512,10 @@
         <v>250</v>
       </c>
       <c r="B120" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C120" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
@@ -14609,10 +14523,10 @@
         <v>250</v>
       </c>
       <c r="B121" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C121" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
@@ -14620,10 +14534,10 @@
         <v>250</v>
       </c>
       <c r="B122" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C122" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
@@ -14631,10 +14545,10 @@
         <v>250</v>
       </c>
       <c r="B123" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C123" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
@@ -14642,10 +14556,10 @@
         <v>250</v>
       </c>
       <c r="B124" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C124" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
@@ -14653,10 +14567,10 @@
         <v>250</v>
       </c>
       <c r="B125" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C125" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
@@ -14664,10 +14578,10 @@
         <v>250</v>
       </c>
       <c r="B126" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C126" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
@@ -14675,10 +14589,10 @@
         <v>250</v>
       </c>
       <c r="B127" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C127" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
@@ -14686,10 +14600,10 @@
         <v>250</v>
       </c>
       <c r="B128" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C128" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
@@ -14697,10 +14611,10 @@
         <v>250</v>
       </c>
       <c r="B129" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C129" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
@@ -14708,10 +14622,10 @@
         <v>250</v>
       </c>
       <c r="B130" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C130" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
@@ -14719,10 +14633,10 @@
         <v>250</v>
       </c>
       <c r="B131" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C131" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
@@ -14730,10 +14644,10 @@
         <v>250</v>
       </c>
       <c r="B132" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C132" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
@@ -14741,10 +14655,10 @@
         <v>250</v>
       </c>
       <c r="B133" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C133" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
@@ -14752,10 +14666,10 @@
         <v>250</v>
       </c>
       <c r="B134" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C134" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
@@ -14763,10 +14677,10 @@
         <v>250</v>
       </c>
       <c r="B135" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C135" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
@@ -14774,10 +14688,10 @@
         <v>250</v>
       </c>
       <c r="B136" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C136" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
@@ -14785,10 +14699,10 @@
         <v>250</v>
       </c>
       <c r="B137" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C137" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
@@ -14796,10 +14710,10 @@
         <v>250</v>
       </c>
       <c r="B138" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C138" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
@@ -14807,10 +14721,10 @@
         <v>250</v>
       </c>
       <c r="B139" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C139" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
@@ -14818,10 +14732,10 @@
         <v>250</v>
       </c>
       <c r="B140" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C140" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
@@ -14829,10 +14743,10 @@
         <v>250</v>
       </c>
       <c r="B141" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C141" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
@@ -14840,10 +14754,10 @@
         <v>250</v>
       </c>
       <c r="B142" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C142" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
@@ -14851,10 +14765,10 @@
         <v>250</v>
       </c>
       <c r="B143" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C143" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
@@ -14862,10 +14776,10 @@
         <v>250</v>
       </c>
       <c r="B144" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C144" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
@@ -14873,10 +14787,10 @@
         <v>250</v>
       </c>
       <c r="B145" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="C145" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
@@ -14884,10 +14798,10 @@
         <v>250</v>
       </c>
       <c r="B146" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C146" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
@@ -14895,10 +14809,10 @@
         <v>250</v>
       </c>
       <c r="B147" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C147" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
@@ -14906,10 +14820,10 @@
         <v>250</v>
       </c>
       <c r="B148" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C148" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
@@ -14917,10 +14831,10 @@
         <v>250</v>
       </c>
       <c r="B149" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="C149" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
@@ -14928,10 +14842,10 @@
         <v>250</v>
       </c>
       <c r="B150" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C150" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
@@ -14939,10 +14853,10 @@
         <v>250</v>
       </c>
       <c r="B151" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C151" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
@@ -14950,10 +14864,10 @@
         <v>250</v>
       </c>
       <c r="B152" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C152" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
@@ -14961,10 +14875,10 @@
         <v>250</v>
       </c>
       <c r="B153" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C153" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
@@ -14972,10 +14886,10 @@
         <v>250</v>
       </c>
       <c r="B154" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C154" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
@@ -14983,10 +14897,10 @@
         <v>250</v>
       </c>
       <c r="B155" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C155" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
@@ -14994,10 +14908,10 @@
         <v>250</v>
       </c>
       <c r="B156" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C156" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
@@ -15005,10 +14919,10 @@
         <v>250</v>
       </c>
       <c r="B157" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="C157" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
@@ -15016,10 +14930,10 @@
         <v>250</v>
       </c>
       <c r="B158" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C158" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
@@ -15027,10 +14941,10 @@
         <v>250</v>
       </c>
       <c r="B159" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C159" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
@@ -15038,10 +14952,10 @@
         <v>250</v>
       </c>
       <c r="B160" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C160" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
@@ -15049,10 +14963,10 @@
         <v>250</v>
       </c>
       <c r="B161" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C161" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
@@ -15060,10 +14974,10 @@
         <v>250</v>
       </c>
       <c r="B162" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C162" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
@@ -15071,10 +14985,10 @@
         <v>250</v>
       </c>
       <c r="B163" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C163" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
@@ -15082,10 +14996,10 @@
         <v>250</v>
       </c>
       <c r="B164" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C164" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
@@ -15093,10 +15007,10 @@
         <v>250</v>
       </c>
       <c r="B165" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C165" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
@@ -15104,10 +15018,10 @@
         <v>250</v>
       </c>
       <c r="B166" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C166" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
@@ -15115,10 +15029,10 @@
         <v>250</v>
       </c>
       <c r="B167" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C167" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
@@ -15126,10 +15040,10 @@
         <v>250</v>
       </c>
       <c r="B168" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C168" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
@@ -15137,32 +15051,10 @@
         <v>250</v>
       </c>
       <c r="B169" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C169" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A170" t="s">
-        <v>250</v>
-      </c>
-      <c r="B170" t="s">
-        <v>330</v>
-      </c>
-      <c r="C170" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A171" t="s">
-        <v>250</v>
-      </c>
-      <c r="B171" t="s">
-        <v>331</v>
-      </c>
-      <c r="C171" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update settings for full nodal detailed modelling
</commit_message>
<xml_diff>
--- a/spine_rts-gmlc/datasets/branch.xlsx
+++ b/spine_rts-gmlc/datasets/branch.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="branch" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="337">
   <si>
     <t>UID</t>
   </si>
@@ -1034,6 +1034,9 @@
   </si>
   <si>
     <t>connection__to_node</t>
+  </si>
+  <si>
+    <t>313_HEAD_STORAGE</t>
   </si>
 </sst>
 </file>
@@ -11253,7 +11256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -12160,10 +12163,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C85"/>
+  <dimension ref="A1:C86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12189,7 +12192,7 @@
         <v>243</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>336</v>
       </c>
       <c r="C2" t="s">
         <v>244</v>
@@ -12200,7 +12203,7 @@
         <v>243</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C3" t="s">
         <v>244</v>
@@ -12211,7 +12214,7 @@
         <v>243</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C4" t="s">
         <v>244</v>
@@ -12222,7 +12225,7 @@
         <v>243</v>
       </c>
       <c r="B5" t="s">
-        <v>247</v>
+        <v>146</v>
       </c>
       <c r="C5" t="s">
         <v>244</v>
@@ -12233,7 +12236,7 @@
         <v>243</v>
       </c>
       <c r="B6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C6" t="s">
         <v>244</v>
@@ -12244,7 +12247,7 @@
         <v>243</v>
       </c>
       <c r="B7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C7" t="s">
         <v>244</v>
@@ -12255,7 +12258,7 @@
         <v>243</v>
       </c>
       <c r="B8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C8" t="s">
         <v>244</v>
@@ -12266,7 +12269,7 @@
         <v>243</v>
       </c>
       <c r="B9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C9" t="s">
         <v>244</v>
@@ -12277,7 +12280,7 @@
         <v>243</v>
       </c>
       <c r="B10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C10" t="s">
         <v>244</v>
@@ -12288,7 +12291,7 @@
         <v>243</v>
       </c>
       <c r="B11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C11" t="s">
         <v>244</v>
@@ -12299,7 +12302,7 @@
         <v>243</v>
       </c>
       <c r="B12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C12" t="s">
         <v>244</v>
@@ -12310,7 +12313,7 @@
         <v>243</v>
       </c>
       <c r="B13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C13" t="s">
         <v>244</v>
@@ -12321,7 +12324,7 @@
         <v>243</v>
       </c>
       <c r="B14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C14" t="s">
         <v>244</v>
@@ -12332,7 +12335,7 @@
         <v>243</v>
       </c>
       <c r="B15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C15" t="s">
         <v>244</v>
@@ -12343,7 +12346,7 @@
         <v>243</v>
       </c>
       <c r="B16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C16" t="s">
         <v>244</v>
@@ -12354,7 +12357,7 @@
         <v>243</v>
       </c>
       <c r="B17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C17" t="s">
         <v>244</v>
@@ -12365,7 +12368,7 @@
         <v>243</v>
       </c>
       <c r="B18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C18" t="s">
         <v>244</v>
@@ -12376,7 +12379,7 @@
         <v>243</v>
       </c>
       <c r="B19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C19" t="s">
         <v>244</v>
@@ -12387,7 +12390,7 @@
         <v>243</v>
       </c>
       <c r="B20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C20" t="s">
         <v>244</v>
@@ -12398,7 +12401,7 @@
         <v>243</v>
       </c>
       <c r="B21" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C21" t="s">
         <v>244</v>
@@ -12409,7 +12412,7 @@
         <v>243</v>
       </c>
       <c r="B22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C22" t="s">
         <v>244</v>
@@ -12420,7 +12423,7 @@
         <v>243</v>
       </c>
       <c r="B23" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C23" t="s">
         <v>244</v>
@@ -12431,7 +12434,7 @@
         <v>243</v>
       </c>
       <c r="B24" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C24" t="s">
         <v>244</v>
@@ -12442,7 +12445,7 @@
         <v>243</v>
       </c>
       <c r="B25" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C25" t="s">
         <v>244</v>
@@ -12453,7 +12456,7 @@
         <v>243</v>
       </c>
       <c r="B26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C26" t="s">
         <v>244</v>
@@ -12464,7 +12467,7 @@
         <v>243</v>
       </c>
       <c r="B27" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C27" t="s">
         <v>244</v>
@@ -12475,7 +12478,7 @@
         <v>243</v>
       </c>
       <c r="B28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C28" t="s">
         <v>244</v>
@@ -12486,7 +12489,7 @@
         <v>243</v>
       </c>
       <c r="B29" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C29" t="s">
         <v>244</v>
@@ -12497,7 +12500,7 @@
         <v>243</v>
       </c>
       <c r="B30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C30" t="s">
         <v>244</v>
@@ -12508,7 +12511,7 @@
         <v>243</v>
       </c>
       <c r="B31" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C31" t="s">
         <v>244</v>
@@ -12519,7 +12522,7 @@
         <v>243</v>
       </c>
       <c r="B32" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C32" t="s">
         <v>244</v>
@@ -12530,7 +12533,7 @@
         <v>243</v>
       </c>
       <c r="B33" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C33" t="s">
         <v>244</v>
@@ -12541,7 +12544,7 @@
         <v>243</v>
       </c>
       <c r="B34" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C34" t="s">
         <v>244</v>
@@ -12552,7 +12555,7 @@
         <v>243</v>
       </c>
       <c r="B35" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C35" t="s">
         <v>244</v>
@@ -12563,7 +12566,7 @@
         <v>243</v>
       </c>
       <c r="B36" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C36" t="s">
         <v>244</v>
@@ -12574,7 +12577,7 @@
         <v>243</v>
       </c>
       <c r="B37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C37" t="s">
         <v>244</v>
@@ -12585,7 +12588,7 @@
         <v>243</v>
       </c>
       <c r="B38" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C38" t="s">
         <v>244</v>
@@ -12596,7 +12599,7 @@
         <v>243</v>
       </c>
       <c r="B39" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C39" t="s">
         <v>244</v>
@@ -12607,7 +12610,7 @@
         <v>243</v>
       </c>
       <c r="B40" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C40" t="s">
         <v>244</v>
@@ -12618,7 +12621,7 @@
         <v>243</v>
       </c>
       <c r="B41" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C41" t="s">
         <v>244</v>
@@ -12629,7 +12632,7 @@
         <v>243</v>
       </c>
       <c r="B42" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C42" t="s">
         <v>244</v>
@@ -12640,7 +12643,7 @@
         <v>243</v>
       </c>
       <c r="B43" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C43" t="s">
         <v>244</v>
@@ -12651,7 +12654,7 @@
         <v>243</v>
       </c>
       <c r="B44" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C44" t="s">
         <v>244</v>
@@ -12662,7 +12665,7 @@
         <v>243</v>
       </c>
       <c r="B45" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C45" t="s">
         <v>244</v>
@@ -12673,7 +12676,7 @@
         <v>243</v>
       </c>
       <c r="B46" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C46" t="s">
         <v>244</v>
@@ -12684,7 +12687,7 @@
         <v>243</v>
       </c>
       <c r="B47" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C47" t="s">
         <v>244</v>
@@ -12695,7 +12698,7 @@
         <v>243</v>
       </c>
       <c r="B48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C48" t="s">
         <v>244</v>
@@ -12706,7 +12709,7 @@
         <v>243</v>
       </c>
       <c r="B49" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C49" t="s">
         <v>244</v>
@@ -12717,7 +12720,7 @@
         <v>243</v>
       </c>
       <c r="B50" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C50" t="s">
         <v>244</v>
@@ -12728,7 +12731,7 @@
         <v>243</v>
       </c>
       <c r="B51" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C51" t="s">
         <v>244</v>
@@ -12739,7 +12742,7 @@
         <v>243</v>
       </c>
       <c r="B52" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C52" t="s">
         <v>244</v>
@@ -12750,7 +12753,7 @@
         <v>243</v>
       </c>
       <c r="B53" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C53" t="s">
         <v>244</v>
@@ -12761,7 +12764,7 @@
         <v>243</v>
       </c>
       <c r="B54" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C54" t="s">
         <v>244</v>
@@ -12772,7 +12775,7 @@
         <v>243</v>
       </c>
       <c r="B55" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C55" t="s">
         <v>244</v>
@@ -12783,7 +12786,7 @@
         <v>243</v>
       </c>
       <c r="B56" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C56" t="s">
         <v>244</v>
@@ -12794,7 +12797,7 @@
         <v>243</v>
       </c>
       <c r="B57" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C57" t="s">
         <v>244</v>
@@ -12805,7 +12808,7 @@
         <v>243</v>
       </c>
       <c r="B58" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C58" t="s">
         <v>244</v>
@@ -12816,7 +12819,7 @@
         <v>243</v>
       </c>
       <c r="B59" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C59" t="s">
         <v>244</v>
@@ -12827,7 +12830,7 @@
         <v>243</v>
       </c>
       <c r="B60" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C60" t="s">
         <v>244</v>
@@ -12838,7 +12841,7 @@
         <v>243</v>
       </c>
       <c r="B61" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C61" t="s">
         <v>244</v>
@@ -12849,7 +12852,7 @@
         <v>243</v>
       </c>
       <c r="B62" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C62" t="s">
         <v>244</v>
@@ -12860,7 +12863,7 @@
         <v>243</v>
       </c>
       <c r="B63" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C63" t="s">
         <v>244</v>
@@ -12871,7 +12874,7 @@
         <v>243</v>
       </c>
       <c r="B64" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C64" t="s">
         <v>244</v>
@@ -12882,7 +12885,7 @@
         <v>243</v>
       </c>
       <c r="B65" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C65" t="s">
         <v>244</v>
@@ -12893,7 +12896,7 @@
         <v>243</v>
       </c>
       <c r="B66" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C66" t="s">
         <v>244</v>
@@ -12904,7 +12907,7 @@
         <v>243</v>
       </c>
       <c r="B67" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C67" t="s">
         <v>244</v>
@@ -12915,7 +12918,7 @@
         <v>243</v>
       </c>
       <c r="B68" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C68" t="s">
         <v>244</v>
@@ -12926,7 +12929,7 @@
         <v>243</v>
       </c>
       <c r="B69" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C69" t="s">
         <v>244</v>
@@ -12937,7 +12940,7 @@
         <v>243</v>
       </c>
       <c r="B70" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C70" t="s">
         <v>244</v>
@@ -12948,7 +12951,7 @@
         <v>243</v>
       </c>
       <c r="B71" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C71" t="s">
         <v>244</v>
@@ -12959,7 +12962,7 @@
         <v>243</v>
       </c>
       <c r="B72" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C72" t="s">
         <v>244</v>
@@ -12970,7 +12973,7 @@
         <v>243</v>
       </c>
       <c r="B73" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C73" t="s">
         <v>244</v>
@@ -12981,7 +12984,7 @@
         <v>243</v>
       </c>
       <c r="B74" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C74" t="s">
         <v>244</v>
@@ -12992,7 +12995,7 @@
         <v>243</v>
       </c>
       <c r="B75" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C75" t="s">
         <v>244</v>
@@ -13003,7 +13006,7 @@
         <v>243</v>
       </c>
       <c r="B76" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C76" t="s">
         <v>244</v>
@@ -13014,7 +13017,7 @@
         <v>243</v>
       </c>
       <c r="B77" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C77" t="s">
         <v>244</v>
@@ -13025,7 +13028,7 @@
         <v>243</v>
       </c>
       <c r="B78" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C78" t="s">
         <v>244</v>
@@ -13036,7 +13039,7 @@
         <v>243</v>
       </c>
       <c r="B79" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C79" t="s">
         <v>244</v>
@@ -13047,7 +13050,7 @@
         <v>243</v>
       </c>
       <c r="B80" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C80" t="s">
         <v>244</v>
@@ -13058,7 +13061,7 @@
         <v>243</v>
       </c>
       <c r="B81" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C81" t="s">
         <v>244</v>
@@ -13069,7 +13072,7 @@
         <v>243</v>
       </c>
       <c r="B82" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C82" t="s">
         <v>244</v>
@@ -13080,7 +13083,7 @@
         <v>243</v>
       </c>
       <c r="B83" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C83" t="s">
         <v>244</v>
@@ -13091,7 +13094,7 @@
         <v>243</v>
       </c>
       <c r="B84" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C84" t="s">
         <v>244</v>
@@ -13102,9 +13105,20 @@
         <v>243</v>
       </c>
       <c r="B85" t="s">
+        <v>326</v>
+      </c>
+      <c r="C85" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>243</v>
+      </c>
+      <c r="B86" t="s">
         <v>327</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C86" t="s">
         <v>244</v>
       </c>
     </row>
@@ -13115,10 +13129,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C169"/>
+  <dimension ref="A1:C171"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89:XFD89"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87:C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13144,7 +13158,7 @@
         <v>246</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>336</v>
       </c>
       <c r="C2" t="s">
         <v>330</v>
@@ -13155,7 +13169,7 @@
         <v>246</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C3" t="s">
         <v>330</v>
@@ -13166,7 +13180,7 @@
         <v>246</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C4" t="s">
         <v>330</v>
@@ -13177,7 +13191,7 @@
         <v>246</v>
       </c>
       <c r="B5" t="s">
-        <v>247</v>
+        <v>146</v>
       </c>
       <c r="C5" t="s">
         <v>330</v>
@@ -13188,7 +13202,7 @@
         <v>246</v>
       </c>
       <c r="B6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C6" t="s">
         <v>330</v>
@@ -13199,7 +13213,7 @@
         <v>246</v>
       </c>
       <c r="B7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C7" t="s">
         <v>330</v>
@@ -13210,7 +13224,7 @@
         <v>246</v>
       </c>
       <c r="B8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C8" t="s">
         <v>330</v>
@@ -13221,7 +13235,7 @@
         <v>246</v>
       </c>
       <c r="B9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C9" t="s">
         <v>330</v>
@@ -13232,7 +13246,7 @@
         <v>246</v>
       </c>
       <c r="B10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C10" t="s">
         <v>330</v>
@@ -13243,7 +13257,7 @@
         <v>246</v>
       </c>
       <c r="B11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C11" t="s">
         <v>330</v>
@@ -13254,7 +13268,7 @@
         <v>246</v>
       </c>
       <c r="B12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C12" t="s">
         <v>330</v>
@@ -13265,7 +13279,7 @@
         <v>246</v>
       </c>
       <c r="B13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C13" t="s">
         <v>330</v>
@@ -13276,7 +13290,7 @@
         <v>246</v>
       </c>
       <c r="B14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C14" t="s">
         <v>330</v>
@@ -13287,7 +13301,7 @@
         <v>246</v>
       </c>
       <c r="B15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C15" t="s">
         <v>330</v>
@@ -13298,7 +13312,7 @@
         <v>246</v>
       </c>
       <c r="B16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C16" t="s">
         <v>330</v>
@@ -13309,7 +13323,7 @@
         <v>246</v>
       </c>
       <c r="B17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C17" t="s">
         <v>330</v>
@@ -13320,7 +13334,7 @@
         <v>246</v>
       </c>
       <c r="B18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C18" t="s">
         <v>330</v>
@@ -13331,7 +13345,7 @@
         <v>246</v>
       </c>
       <c r="B19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C19" t="s">
         <v>330</v>
@@ -13342,7 +13356,7 @@
         <v>246</v>
       </c>
       <c r="B20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C20" t="s">
         <v>330</v>
@@ -13353,7 +13367,7 @@
         <v>246</v>
       </c>
       <c r="B21" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C21" t="s">
         <v>330</v>
@@ -13364,7 +13378,7 @@
         <v>246</v>
       </c>
       <c r="B22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C22" t="s">
         <v>330</v>
@@ -13375,7 +13389,7 @@
         <v>246</v>
       </c>
       <c r="B23" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C23" t="s">
         <v>330</v>
@@ -13386,7 +13400,7 @@
         <v>246</v>
       </c>
       <c r="B24" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C24" t="s">
         <v>330</v>
@@ -13397,7 +13411,7 @@
         <v>246</v>
       </c>
       <c r="B25" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C25" t="s">
         <v>330</v>
@@ -13408,7 +13422,7 @@
         <v>246</v>
       </c>
       <c r="B26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C26" t="s">
         <v>330</v>
@@ -13419,7 +13433,7 @@
         <v>246</v>
       </c>
       <c r="B27" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C27" t="s">
         <v>330</v>
@@ -13430,7 +13444,7 @@
         <v>246</v>
       </c>
       <c r="B28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C28" t="s">
         <v>330</v>
@@ -13441,7 +13455,7 @@
         <v>246</v>
       </c>
       <c r="B29" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C29" t="s">
         <v>330</v>
@@ -13452,7 +13466,7 @@
         <v>246</v>
       </c>
       <c r="B30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C30" t="s">
         <v>330</v>
@@ -13463,7 +13477,7 @@
         <v>246</v>
       </c>
       <c r="B31" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C31" t="s">
         <v>330</v>
@@ -13474,7 +13488,7 @@
         <v>246</v>
       </c>
       <c r="B32" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C32" t="s">
         <v>330</v>
@@ -13485,7 +13499,7 @@
         <v>246</v>
       </c>
       <c r="B33" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C33" t="s">
         <v>330</v>
@@ -13496,7 +13510,7 @@
         <v>246</v>
       </c>
       <c r="B34" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C34" t="s">
         <v>330</v>
@@ -13507,7 +13521,7 @@
         <v>246</v>
       </c>
       <c r="B35" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C35" t="s">
         <v>330</v>
@@ -13518,7 +13532,7 @@
         <v>246</v>
       </c>
       <c r="B36" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C36" t="s">
         <v>330</v>
@@ -13529,7 +13543,7 @@
         <v>246</v>
       </c>
       <c r="B37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C37" t="s">
         <v>330</v>
@@ -13540,7 +13554,7 @@
         <v>246</v>
       </c>
       <c r="B38" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C38" t="s">
         <v>330</v>
@@ -13551,7 +13565,7 @@
         <v>246</v>
       </c>
       <c r="B39" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C39" t="s">
         <v>330</v>
@@ -13562,7 +13576,7 @@
         <v>246</v>
       </c>
       <c r="B40" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C40" t="s">
         <v>330</v>
@@ -13573,7 +13587,7 @@
         <v>246</v>
       </c>
       <c r="B41" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C41" t="s">
         <v>330</v>
@@ -13584,7 +13598,7 @@
         <v>246</v>
       </c>
       <c r="B42" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C42" t="s">
         <v>330</v>
@@ -13595,7 +13609,7 @@
         <v>246</v>
       </c>
       <c r="B43" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C43" t="s">
         <v>330</v>
@@ -13606,7 +13620,7 @@
         <v>246</v>
       </c>
       <c r="B44" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C44" t="s">
         <v>330</v>
@@ -13617,7 +13631,7 @@
         <v>246</v>
       </c>
       <c r="B45" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C45" t="s">
         <v>330</v>
@@ -13628,7 +13642,7 @@
         <v>246</v>
       </c>
       <c r="B46" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C46" t="s">
         <v>330</v>
@@ -13639,7 +13653,7 @@
         <v>246</v>
       </c>
       <c r="B47" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C47" t="s">
         <v>330</v>
@@ -13650,7 +13664,7 @@
         <v>246</v>
       </c>
       <c r="B48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C48" t="s">
         <v>330</v>
@@ -13661,7 +13675,7 @@
         <v>246</v>
       </c>
       <c r="B49" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C49" t="s">
         <v>330</v>
@@ -13672,7 +13686,7 @@
         <v>246</v>
       </c>
       <c r="B50" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C50" t="s">
         <v>330</v>
@@ -13683,7 +13697,7 @@
         <v>246</v>
       </c>
       <c r="B51" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C51" t="s">
         <v>330</v>
@@ -13694,7 +13708,7 @@
         <v>246</v>
       </c>
       <c r="B52" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C52" t="s">
         <v>330</v>
@@ -13705,7 +13719,7 @@
         <v>246</v>
       </c>
       <c r="B53" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C53" t="s">
         <v>330</v>
@@ -13716,7 +13730,7 @@
         <v>246</v>
       </c>
       <c r="B54" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C54" t="s">
         <v>330</v>
@@ -13727,7 +13741,7 @@
         <v>246</v>
       </c>
       <c r="B55" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C55" t="s">
         <v>330</v>
@@ -13738,7 +13752,7 @@
         <v>246</v>
       </c>
       <c r="B56" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C56" t="s">
         <v>330</v>
@@ -13749,7 +13763,7 @@
         <v>246</v>
       </c>
       <c r="B57" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C57" t="s">
         <v>330</v>
@@ -13760,7 +13774,7 @@
         <v>246</v>
       </c>
       <c r="B58" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C58" t="s">
         <v>330</v>
@@ -13771,7 +13785,7 @@
         <v>246</v>
       </c>
       <c r="B59" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C59" t="s">
         <v>330</v>
@@ -13782,7 +13796,7 @@
         <v>246</v>
       </c>
       <c r="B60" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C60" t="s">
         <v>330</v>
@@ -13793,7 +13807,7 @@
         <v>246</v>
       </c>
       <c r="B61" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C61" t="s">
         <v>330</v>
@@ -13804,7 +13818,7 @@
         <v>246</v>
       </c>
       <c r="B62" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C62" t="s">
         <v>330</v>
@@ -13815,7 +13829,7 @@
         <v>246</v>
       </c>
       <c r="B63" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C63" t="s">
         <v>330</v>
@@ -13826,7 +13840,7 @@
         <v>246</v>
       </c>
       <c r="B64" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C64" t="s">
         <v>330</v>
@@ -13837,7 +13851,7 @@
         <v>246</v>
       </c>
       <c r="B65" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C65" t="s">
         <v>330</v>
@@ -13848,7 +13862,7 @@
         <v>246</v>
       </c>
       <c r="B66" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C66" t="s">
         <v>330</v>
@@ -13859,7 +13873,7 @@
         <v>246</v>
       </c>
       <c r="B67" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C67" t="s">
         <v>330</v>
@@ -13870,7 +13884,7 @@
         <v>246</v>
       </c>
       <c r="B68" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C68" t="s">
         <v>330</v>
@@ -13881,7 +13895,7 @@
         <v>246</v>
       </c>
       <c r="B69" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C69" t="s">
         <v>330</v>
@@ -13892,7 +13906,7 @@
         <v>246</v>
       </c>
       <c r="B70" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C70" t="s">
         <v>330</v>
@@ -13903,7 +13917,7 @@
         <v>246</v>
       </c>
       <c r="B71" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C71" t="s">
         <v>330</v>
@@ -13914,7 +13928,7 @@
         <v>246</v>
       </c>
       <c r="B72" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C72" t="s">
         <v>330</v>
@@ -13925,7 +13939,7 @@
         <v>246</v>
       </c>
       <c r="B73" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C73" t="s">
         <v>330</v>
@@ -13936,7 +13950,7 @@
         <v>246</v>
       </c>
       <c r="B74" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C74" t="s">
         <v>330</v>
@@ -13947,7 +13961,7 @@
         <v>246</v>
       </c>
       <c r="B75" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C75" t="s">
         <v>330</v>
@@ -13958,7 +13972,7 @@
         <v>246</v>
       </c>
       <c r="B76" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C76" t="s">
         <v>330</v>
@@ -13969,7 +13983,7 @@
         <v>246</v>
       </c>
       <c r="B77" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C77" t="s">
         <v>330</v>
@@ -13980,7 +13994,7 @@
         <v>246</v>
       </c>
       <c r="B78" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C78" t="s">
         <v>330</v>
@@ -13991,7 +14005,7 @@
         <v>246</v>
       </c>
       <c r="B79" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C79" t="s">
         <v>330</v>
@@ -14002,7 +14016,7 @@
         <v>246</v>
       </c>
       <c r="B80" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C80" t="s">
         <v>330</v>
@@ -14013,7 +14027,7 @@
         <v>246</v>
       </c>
       <c r="B81" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C81" t="s">
         <v>330</v>
@@ -14024,7 +14038,7 @@
         <v>246</v>
       </c>
       <c r="B82" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C82" t="s">
         <v>330</v>
@@ -14035,7 +14049,7 @@
         <v>246</v>
       </c>
       <c r="B83" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C83" t="s">
         <v>330</v>
@@ -14046,7 +14060,7 @@
         <v>246</v>
       </c>
       <c r="B84" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C84" t="s">
         <v>330</v>
@@ -14057,7 +14071,7 @@
         <v>246</v>
       </c>
       <c r="B85" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C85" t="s">
         <v>330</v>
@@ -14068,10 +14082,10 @@
         <v>246</v>
       </c>
       <c r="B86" t="s">
-        <v>144</v>
+        <v>327</v>
       </c>
       <c r="C86" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
@@ -14079,7 +14093,7 @@
         <v>246</v>
       </c>
       <c r="B87" t="s">
-        <v>145</v>
+        <v>336</v>
       </c>
       <c r="C87" t="s">
         <v>331</v>
@@ -14090,7 +14104,7 @@
         <v>246</v>
       </c>
       <c r="B88" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C88" t="s">
         <v>331</v>
@@ -14101,7 +14115,7 @@
         <v>246</v>
       </c>
       <c r="B89" t="s">
-        <v>247</v>
+        <v>145</v>
       </c>
       <c r="C89" t="s">
         <v>331</v>
@@ -14112,7 +14126,7 @@
         <v>246</v>
       </c>
       <c r="B90" t="s">
-        <v>248</v>
+        <v>146</v>
       </c>
       <c r="C90" t="s">
         <v>331</v>
@@ -14123,7 +14137,7 @@
         <v>246</v>
       </c>
       <c r="B91" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C91" t="s">
         <v>331</v>
@@ -14134,7 +14148,7 @@
         <v>246</v>
       </c>
       <c r="B92" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C92" t="s">
         <v>331</v>
@@ -14145,7 +14159,7 @@
         <v>246</v>
       </c>
       <c r="B93" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C93" t="s">
         <v>331</v>
@@ -14156,7 +14170,7 @@
         <v>246</v>
       </c>
       <c r="B94" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C94" t="s">
         <v>331</v>
@@ -14167,7 +14181,7 @@
         <v>246</v>
       </c>
       <c r="B95" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C95" t="s">
         <v>331</v>
@@ -14178,7 +14192,7 @@
         <v>246</v>
       </c>
       <c r="B96" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C96" t="s">
         <v>331</v>
@@ -14189,7 +14203,7 @@
         <v>246</v>
       </c>
       <c r="B97" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C97" t="s">
         <v>331</v>
@@ -14200,7 +14214,7 @@
         <v>246</v>
       </c>
       <c r="B98" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C98" t="s">
         <v>331</v>
@@ -14211,7 +14225,7 @@
         <v>246</v>
       </c>
       <c r="B99" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C99" t="s">
         <v>331</v>
@@ -14222,7 +14236,7 @@
         <v>246</v>
       </c>
       <c r="B100" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C100" t="s">
         <v>331</v>
@@ -14233,7 +14247,7 @@
         <v>246</v>
       </c>
       <c r="B101" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C101" t="s">
         <v>331</v>
@@ -14244,7 +14258,7 @@
         <v>246</v>
       </c>
       <c r="B102" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C102" t="s">
         <v>331</v>
@@ -14255,7 +14269,7 @@
         <v>246</v>
       </c>
       <c r="B103" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C103" t="s">
         <v>331</v>
@@ -14266,7 +14280,7 @@
         <v>246</v>
       </c>
       <c r="B104" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C104" t="s">
         <v>331</v>
@@ -14277,7 +14291,7 @@
         <v>246</v>
       </c>
       <c r="B105" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C105" t="s">
         <v>331</v>
@@ -14288,7 +14302,7 @@
         <v>246</v>
       </c>
       <c r="B106" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C106" t="s">
         <v>331</v>
@@ -14299,7 +14313,7 @@
         <v>246</v>
       </c>
       <c r="B107" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C107" t="s">
         <v>331</v>
@@ -14310,7 +14324,7 @@
         <v>246</v>
       </c>
       <c r="B108" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C108" t="s">
         <v>331</v>
@@ -14321,7 +14335,7 @@
         <v>246</v>
       </c>
       <c r="B109" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C109" t="s">
         <v>331</v>
@@ -14332,7 +14346,7 @@
         <v>246</v>
       </c>
       <c r="B110" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C110" t="s">
         <v>331</v>
@@ -14343,7 +14357,7 @@
         <v>246</v>
       </c>
       <c r="B111" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C111" t="s">
         <v>331</v>
@@ -14354,7 +14368,7 @@
         <v>246</v>
       </c>
       <c r="B112" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C112" t="s">
         <v>331</v>
@@ -14365,7 +14379,7 @@
         <v>246</v>
       </c>
       <c r="B113" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C113" t="s">
         <v>331</v>
@@ -14376,7 +14390,7 @@
         <v>246</v>
       </c>
       <c r="B114" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C114" t="s">
         <v>331</v>
@@ -14387,7 +14401,7 @@
         <v>246</v>
       </c>
       <c r="B115" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C115" t="s">
         <v>331</v>
@@ -14398,7 +14412,7 @@
         <v>246</v>
       </c>
       <c r="B116" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C116" t="s">
         <v>331</v>
@@ -14409,7 +14423,7 @@
         <v>246</v>
       </c>
       <c r="B117" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C117" t="s">
         <v>331</v>
@@ -14420,7 +14434,7 @@
         <v>246</v>
       </c>
       <c r="B118" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C118" t="s">
         <v>331</v>
@@ -14431,7 +14445,7 @@
         <v>246</v>
       </c>
       <c r="B119" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C119" t="s">
         <v>331</v>
@@ -14442,7 +14456,7 @@
         <v>246</v>
       </c>
       <c r="B120" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C120" t="s">
         <v>331</v>
@@ -14453,7 +14467,7 @@
         <v>246</v>
       </c>
       <c r="B121" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C121" t="s">
         <v>331</v>
@@ -14464,7 +14478,7 @@
         <v>246</v>
       </c>
       <c r="B122" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C122" t="s">
         <v>331</v>
@@ -14475,7 +14489,7 @@
         <v>246</v>
       </c>
       <c r="B123" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C123" t="s">
         <v>331</v>
@@ -14486,7 +14500,7 @@
         <v>246</v>
       </c>
       <c r="B124" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C124" t="s">
         <v>331</v>
@@ -14497,7 +14511,7 @@
         <v>246</v>
       </c>
       <c r="B125" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C125" t="s">
         <v>331</v>
@@ -14508,7 +14522,7 @@
         <v>246</v>
       </c>
       <c r="B126" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C126" t="s">
         <v>331</v>
@@ -14519,7 +14533,7 @@
         <v>246</v>
       </c>
       <c r="B127" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C127" t="s">
         <v>331</v>
@@ -14530,7 +14544,7 @@
         <v>246</v>
       </c>
       <c r="B128" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C128" t="s">
         <v>331</v>
@@ -14541,7 +14555,7 @@
         <v>246</v>
       </c>
       <c r="B129" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C129" t="s">
         <v>331</v>
@@ -14552,7 +14566,7 @@
         <v>246</v>
       </c>
       <c r="B130" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C130" t="s">
         <v>331</v>
@@ -14563,7 +14577,7 @@
         <v>246</v>
       </c>
       <c r="B131" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C131" t="s">
         <v>331</v>
@@ -14574,7 +14588,7 @@
         <v>246</v>
       </c>
       <c r="B132" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C132" t="s">
         <v>331</v>
@@ -14585,7 +14599,7 @@
         <v>246</v>
       </c>
       <c r="B133" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C133" t="s">
         <v>331</v>
@@ -14596,7 +14610,7 @@
         <v>246</v>
       </c>
       <c r="B134" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C134" t="s">
         <v>331</v>
@@ -14607,7 +14621,7 @@
         <v>246</v>
       </c>
       <c r="B135" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C135" t="s">
         <v>331</v>
@@ -14618,7 +14632,7 @@
         <v>246</v>
       </c>
       <c r="B136" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C136" t="s">
         <v>331</v>
@@ -14629,7 +14643,7 @@
         <v>246</v>
       </c>
       <c r="B137" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C137" t="s">
         <v>331</v>
@@ -14640,7 +14654,7 @@
         <v>246</v>
       </c>
       <c r="B138" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C138" t="s">
         <v>331</v>
@@ -14651,7 +14665,7 @@
         <v>246</v>
       </c>
       <c r="B139" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C139" t="s">
         <v>331</v>
@@ -14662,7 +14676,7 @@
         <v>246</v>
       </c>
       <c r="B140" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C140" t="s">
         <v>331</v>
@@ -14673,7 +14687,7 @@
         <v>246</v>
       </c>
       <c r="B141" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C141" t="s">
         <v>331</v>
@@ -14684,7 +14698,7 @@
         <v>246</v>
       </c>
       <c r="B142" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C142" t="s">
         <v>331</v>
@@ -14695,7 +14709,7 @@
         <v>246</v>
       </c>
       <c r="B143" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C143" t="s">
         <v>331</v>
@@ -14706,7 +14720,7 @@
         <v>246</v>
       </c>
       <c r="B144" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C144" t="s">
         <v>331</v>
@@ -14717,7 +14731,7 @@
         <v>246</v>
       </c>
       <c r="B145" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C145" t="s">
         <v>331</v>
@@ -14728,7 +14742,7 @@
         <v>246</v>
       </c>
       <c r="B146" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C146" t="s">
         <v>331</v>
@@ -14739,7 +14753,7 @@
         <v>246</v>
       </c>
       <c r="B147" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C147" t="s">
         <v>331</v>
@@ -14750,7 +14764,7 @@
         <v>246</v>
       </c>
       <c r="B148" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C148" t="s">
         <v>331</v>
@@ -14761,7 +14775,7 @@
         <v>246</v>
       </c>
       <c r="B149" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C149" t="s">
         <v>331</v>
@@ -14772,7 +14786,7 @@
         <v>246</v>
       </c>
       <c r="B150" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C150" t="s">
         <v>331</v>
@@ -14783,7 +14797,7 @@
         <v>246</v>
       </c>
       <c r="B151" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C151" t="s">
         <v>331</v>
@@ -14794,7 +14808,7 @@
         <v>246</v>
       </c>
       <c r="B152" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C152" t="s">
         <v>331</v>
@@ -14805,7 +14819,7 @@
         <v>246</v>
       </c>
       <c r="B153" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C153" t="s">
         <v>331</v>
@@ -14816,7 +14830,7 @@
         <v>246</v>
       </c>
       <c r="B154" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C154" t="s">
         <v>331</v>
@@ -14827,7 +14841,7 @@
         <v>246</v>
       </c>
       <c r="B155" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C155" t="s">
         <v>331</v>
@@ -14838,7 +14852,7 @@
         <v>246</v>
       </c>
       <c r="B156" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C156" t="s">
         <v>331</v>
@@ -14849,7 +14863,7 @@
         <v>246</v>
       </c>
       <c r="B157" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C157" t="s">
         <v>331</v>
@@ -14860,7 +14874,7 @@
         <v>246</v>
       </c>
       <c r="B158" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C158" t="s">
         <v>331</v>
@@ -14871,7 +14885,7 @@
         <v>246</v>
       </c>
       <c r="B159" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C159" t="s">
         <v>331</v>
@@ -14882,7 +14896,7 @@
         <v>246</v>
       </c>
       <c r="B160" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C160" t="s">
         <v>331</v>
@@ -14893,7 +14907,7 @@
         <v>246</v>
       </c>
       <c r="B161" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C161" t="s">
         <v>331</v>
@@ -14904,7 +14918,7 @@
         <v>246</v>
       </c>
       <c r="B162" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C162" t="s">
         <v>331</v>
@@ -14915,7 +14929,7 @@
         <v>246</v>
       </c>
       <c r="B163" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C163" t="s">
         <v>331</v>
@@ -14926,7 +14940,7 @@
         <v>246</v>
       </c>
       <c r="B164" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C164" t="s">
         <v>331</v>
@@ -14937,7 +14951,7 @@
         <v>246</v>
       </c>
       <c r="B165" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C165" t="s">
         <v>331</v>
@@ -14948,7 +14962,7 @@
         <v>246</v>
       </c>
       <c r="B166" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C166" t="s">
         <v>331</v>
@@ -14959,7 +14973,7 @@
         <v>246</v>
       </c>
       <c r="B167" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C167" t="s">
         <v>331</v>
@@ -14970,7 +14984,7 @@
         <v>246</v>
       </c>
       <c r="B168" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C168" t="s">
         <v>331</v>
@@ -14981,9 +14995,31 @@
         <v>246</v>
       </c>
       <c r="B169" t="s">
+        <v>325</v>
+      </c>
+      <c r="C169" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>246</v>
+      </c>
+      <c r="B170" t="s">
+        <v>326</v>
+      </c>
+      <c r="C170" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>246</v>
+      </c>
+      <c r="B171" t="s">
         <v>327</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C171" t="s">
         <v>331</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update settings for system modelling
</commit_message>
<xml_diff>
--- a/spine_rts-gmlc/datasets/branch.xlsx
+++ b/spine_rts-gmlc/datasets/branch.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="branch" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,12 @@
     <sheet name="rel_node__commodity" sheetId="5" r:id="rId7"/>
     <sheet name="rel_node__temporal_block" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="338">
   <si>
     <t>UID</t>
   </si>
@@ -1037,6 +1037,9 @@
   </si>
   <si>
     <t>313_HEAD_STORAGE</t>
+  </si>
+  <si>
+    <t>1-3-DC1</t>
   </si>
 </sst>
 </file>
@@ -11185,10 +11188,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11247,6 +11250,14 @@
         <v>143</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" t="s">
+        <v>337</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11257,7 +11268,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11274,7 +11285,7 @@
     <col min="11" max="11" width="22.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>134</v>
       </c>
@@ -11291,12 +11302,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>334</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>239</v>
+      <c r="B2" s="2" t="s">
+        <v>337</v>
       </c>
       <c r="C2" t="s">
         <v>144</v>
@@ -11305,15 +11316,15 @@
         <v>332</v>
       </c>
       <c r="E2">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>335</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>239</v>
+      <c r="B3" s="2" t="s">
+        <v>337</v>
       </c>
       <c r="C3" t="s">
         <v>144</v>
@@ -11322,49 +11333,52 @@
         <v>332</v>
       </c>
       <c r="E3">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>334</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>239</v>
+      <c r="B4" s="2" t="s">
+        <v>337</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D4" t="s">
         <v>332</v>
       </c>
       <c r="E4">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>335</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>239</v>
+      <c r="B5" s="2" t="s">
+        <v>337</v>
       </c>
       <c r="C5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D5" t="s">
         <v>332</v>
       </c>
       <c r="E5">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>334</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C6" t="s">
         <v>144</v>
@@ -11373,15 +11387,15 @@
         <v>332</v>
       </c>
       <c r="E6">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>335</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C7" t="s">
         <v>144</v>
@@ -11390,15 +11404,15 @@
         <v>332</v>
       </c>
       <c r="E7">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>334</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C8" t="s">
         <v>145</v>
@@ -11407,15 +11421,15 @@
         <v>332</v>
       </c>
       <c r="E8">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>335</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C9" t="s">
         <v>145</v>
@@ -11424,15 +11438,15 @@
         <v>332</v>
       </c>
       <c r="E9">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>334</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C10" t="s">
         <v>144</v>
@@ -11444,12 +11458,12 @@
         <v>500</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>335</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C11" t="s">
         <v>144</v>
@@ -11461,12 +11475,12 @@
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>334</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C12" t="s">
         <v>145</v>
@@ -11478,12 +11492,12 @@
         <v>500</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>335</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C13" t="s">
         <v>145</v>
@@ -11495,12 +11509,12 @@
         <v>500</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>334</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>142</v>
+      <c r="B14" s="1" t="s">
+        <v>241</v>
       </c>
       <c r="C14" t="s">
         <v>144</v>
@@ -11512,12 +11526,12 @@
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>335</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>142</v>
+      <c r="B15" s="1" t="s">
+        <v>241</v>
       </c>
       <c r="C15" t="s">
         <v>144</v>
@@ -11529,15 +11543,15 @@
         <v>500</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>334</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>142</v>
+      <c r="B16" s="1" t="s">
+        <v>241</v>
       </c>
       <c r="C16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D16" t="s">
         <v>332</v>
@@ -11550,11 +11564,11 @@
       <c r="A17" t="s">
         <v>335</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>142</v>
+      <c r="B17" s="1" t="s">
+        <v>241</v>
       </c>
       <c r="C17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D17" t="s">
         <v>332</v>
@@ -11568,10 +11582,10 @@
         <v>334</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D18" t="s">
         <v>332</v>
@@ -11585,10 +11599,10 @@
         <v>335</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D19" t="s">
         <v>332</v>
@@ -11602,7 +11616,7 @@
         <v>334</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C20" t="s">
         <v>146</v>
@@ -11619,7 +11633,7 @@
         <v>335</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C21" t="s">
         <v>146</v>
@@ -11632,19 +11646,72 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B22" s="2"/>
+      <c r="A22" t="s">
+        <v>334</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C22" t="s">
+        <v>145</v>
+      </c>
+      <c r="D22" t="s">
+        <v>332</v>
+      </c>
+      <c r="E22">
+        <v>500</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="A23" t="s">
+        <v>335</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23" t="s">
+        <v>145</v>
+      </c>
+      <c r="D23" t="s">
+        <v>332</v>
+      </c>
+      <c r="E23">
+        <v>500</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B24" s="1"/>
-      <c r="H24" s="1"/>
+      <c r="A24" t="s">
+        <v>334</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" t="s">
+        <v>146</v>
+      </c>
+      <c r="D24" t="s">
+        <v>332</v>
+      </c>
+      <c r="E24">
+        <v>500</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="A25" t="s">
+        <v>335</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" t="s">
+        <v>146</v>
+      </c>
+      <c r="D25" t="s">
+        <v>332</v>
+      </c>
+      <c r="E25">
+        <v>500</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B26" s="1"/>
@@ -11724,8 +11791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11955,8 +12022,45 @@
         <v>0.99</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>328</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C12" t="s">
+        <v>144</v>
+      </c>
+      <c r="D12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" t="s">
+        <v>333</v>
+      </c>
+      <c r="F12">
+        <v>0.99</v>
+      </c>
+    </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B13" s="1"/>
+      <c r="A13" t="s">
+        <v>328</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C13" t="s">
+        <v>146</v>
+      </c>
+      <c r="D13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" t="s">
+        <v>333</v>
+      </c>
+      <c r="F13">
+        <v>0.99</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
@@ -12022,10 +12126,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12156,6 +12260,28 @@
         <v>146</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>329</v>
+      </c>
+      <c r="B12" t="s">
+        <v>337</v>
+      </c>
+      <c r="C12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>329</v>
+      </c>
+      <c r="B13" t="s">
+        <v>337</v>
+      </c>
+      <c r="C13" t="s">
+        <v>146</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12165,7 +12291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -13131,8 +13257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87:C87"/>
+    <sheetView topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
update data settings to activate ptdf calculation
</commit_message>
<xml_diff>
--- a/spine_rts-gmlc/datasets/branch.xlsx
+++ b/spine_rts-gmlc/datasets/branch.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="branch" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="337">
   <si>
     <t>UID</t>
   </si>
@@ -1033,6 +1033,9 @@
   </si>
   <si>
     <t>parameter_values</t>
+  </si>
+  <si>
+    <t>energy_carrier</t>
   </si>
 </sst>
 </file>
@@ -11183,7 +11186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -12121,8 +12124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12151,7 +12154,7 @@
         <v>332</v>
       </c>
       <c r="C2" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -12195,7 +12198,7 @@
         <v>244</v>
       </c>
       <c r="C6" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -12206,7 +12209,7 @@
         <v>245</v>
       </c>
       <c r="C7" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -12217,7 +12220,7 @@
         <v>246</v>
       </c>
       <c r="C8" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -12228,7 +12231,7 @@
         <v>247</v>
       </c>
       <c r="C9" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -12239,7 +12242,7 @@
         <v>248</v>
       </c>
       <c r="C10" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -12250,7 +12253,7 @@
         <v>249</v>
       </c>
       <c r="C11" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -12261,7 +12264,7 @@
         <v>250</v>
       </c>
       <c r="C12" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -12272,7 +12275,7 @@
         <v>251</v>
       </c>
       <c r="C13" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -12283,7 +12286,7 @@
         <v>252</v>
       </c>
       <c r="C14" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -12294,7 +12297,7 @@
         <v>253</v>
       </c>
       <c r="C15" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -12305,7 +12308,7 @@
         <v>254</v>
       </c>
       <c r="C16" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -12316,7 +12319,7 @@
         <v>255</v>
       </c>
       <c r="C17" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -12327,7 +12330,7 @@
         <v>256</v>
       </c>
       <c r="C18" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -12338,7 +12341,7 @@
         <v>257</v>
       </c>
       <c r="C19" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -12349,7 +12352,7 @@
         <v>258</v>
       </c>
       <c r="C20" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -12360,7 +12363,7 @@
         <v>259</v>
       </c>
       <c r="C21" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -12371,7 +12374,7 @@
         <v>260</v>
       </c>
       <c r="C22" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -12382,7 +12385,7 @@
         <v>261</v>
       </c>
       <c r="C23" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -12393,7 +12396,7 @@
         <v>262</v>
       </c>
       <c r="C24" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -12404,7 +12407,7 @@
         <v>263</v>
       </c>
       <c r="C25" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -12415,7 +12418,7 @@
         <v>264</v>
       </c>
       <c r="C26" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -12426,7 +12429,7 @@
         <v>265</v>
       </c>
       <c r="C27" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -12437,7 +12440,7 @@
         <v>266</v>
       </c>
       <c r="C28" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -12448,7 +12451,7 @@
         <v>267</v>
       </c>
       <c r="C29" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -12459,7 +12462,7 @@
         <v>268</v>
       </c>
       <c r="C30" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -12470,7 +12473,7 @@
         <v>269</v>
       </c>
       <c r="C31" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -12481,7 +12484,7 @@
         <v>270</v>
       </c>
       <c r="C32" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -12492,7 +12495,7 @@
         <v>271</v>
       </c>
       <c r="C33" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -12503,7 +12506,7 @@
         <v>272</v>
       </c>
       <c r="C34" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -12514,7 +12517,7 @@
         <v>273</v>
       </c>
       <c r="C35" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -12525,7 +12528,7 @@
         <v>274</v>
       </c>
       <c r="C36" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -12536,7 +12539,7 @@
         <v>275</v>
       </c>
       <c r="C37" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -12547,7 +12550,7 @@
         <v>276</v>
       </c>
       <c r="C38" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -12558,7 +12561,7 @@
         <v>277</v>
       </c>
       <c r="C39" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
@@ -12569,7 +12572,7 @@
         <v>278</v>
       </c>
       <c r="C40" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
@@ -12580,7 +12583,7 @@
         <v>279</v>
       </c>
       <c r="C41" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -12591,7 +12594,7 @@
         <v>280</v>
       </c>
       <c r="C42" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
@@ -12602,7 +12605,7 @@
         <v>281</v>
       </c>
       <c r="C43" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -12613,7 +12616,7 @@
         <v>282</v>
       </c>
       <c r="C44" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -12624,7 +12627,7 @@
         <v>283</v>
       </c>
       <c r="C45" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
@@ -12635,7 +12638,7 @@
         <v>284</v>
       </c>
       <c r="C46" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
@@ -12646,7 +12649,7 @@
         <v>285</v>
       </c>
       <c r="C47" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
@@ -12657,7 +12660,7 @@
         <v>286</v>
       </c>
       <c r="C48" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -12668,7 +12671,7 @@
         <v>287</v>
       </c>
       <c r="C49" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -12679,7 +12682,7 @@
         <v>288</v>
       </c>
       <c r="C50" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -12690,7 +12693,7 @@
         <v>289</v>
       </c>
       <c r="C51" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -12701,7 +12704,7 @@
         <v>290</v>
       </c>
       <c r="C52" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
@@ -12712,7 +12715,7 @@
         <v>291</v>
       </c>
       <c r="C53" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
@@ -12723,7 +12726,7 @@
         <v>292</v>
       </c>
       <c r="C54" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -12734,7 +12737,7 @@
         <v>293</v>
       </c>
       <c r="C55" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
@@ -12745,7 +12748,7 @@
         <v>294</v>
       </c>
       <c r="C56" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
@@ -12756,7 +12759,7 @@
         <v>295</v>
       </c>
       <c r="C57" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
@@ -12767,7 +12770,7 @@
         <v>296</v>
       </c>
       <c r="C58" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
@@ -12778,7 +12781,7 @@
         <v>297</v>
       </c>
       <c r="C59" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
@@ -12789,7 +12792,7 @@
         <v>298</v>
       </c>
       <c r="C60" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
@@ -12800,7 +12803,7 @@
         <v>299</v>
       </c>
       <c r="C61" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
@@ -12811,7 +12814,7 @@
         <v>300</v>
       </c>
       <c r="C62" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
@@ -12822,7 +12825,7 @@
         <v>301</v>
       </c>
       <c r="C63" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
@@ -12833,7 +12836,7 @@
         <v>302</v>
       </c>
       <c r="C64" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
@@ -12844,7 +12847,7 @@
         <v>303</v>
       </c>
       <c r="C65" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
@@ -12855,7 +12858,7 @@
         <v>304</v>
       </c>
       <c r="C66" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
@@ -12866,7 +12869,7 @@
         <v>305</v>
       </c>
       <c r="C67" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
@@ -12877,7 +12880,7 @@
         <v>306</v>
       </c>
       <c r="C68" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
@@ -12888,7 +12891,7 @@
         <v>307</v>
       </c>
       <c r="C69" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
@@ -12899,7 +12902,7 @@
         <v>308</v>
       </c>
       <c r="C70" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
@@ -12910,7 +12913,7 @@
         <v>309</v>
       </c>
       <c r="C71" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
@@ -12921,7 +12924,7 @@
         <v>310</v>
       </c>
       <c r="C72" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
@@ -12932,7 +12935,7 @@
         <v>311</v>
       </c>
       <c r="C73" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
@@ -12943,7 +12946,7 @@
         <v>312</v>
       </c>
       <c r="C74" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
@@ -12954,7 +12957,7 @@
         <v>313</v>
       </c>
       <c r="C75" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
@@ -12965,7 +12968,7 @@
         <v>314</v>
       </c>
       <c r="C76" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
@@ -12976,7 +12979,7 @@
         <v>315</v>
       </c>
       <c r="C77" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
@@ -12987,7 +12990,7 @@
         <v>316</v>
       </c>
       <c r="C78" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
@@ -12998,7 +13001,7 @@
         <v>317</v>
       </c>
       <c r="C79" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
@@ -13009,7 +13012,7 @@
         <v>318</v>
       </c>
       <c r="C80" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
@@ -13020,7 +13023,7 @@
         <v>319</v>
       </c>
       <c r="C81" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
@@ -13031,7 +13034,7 @@
         <v>320</v>
       </c>
       <c r="C82" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
@@ -13042,7 +13045,7 @@
         <v>321</v>
       </c>
       <c r="C83" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
@@ -13053,7 +13056,7 @@
         <v>322</v>
       </c>
       <c r="C84" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
@@ -13064,7 +13067,7 @@
         <v>323</v>
       </c>
       <c r="C85" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
@@ -13075,7 +13078,7 @@
         <v>324</v>
       </c>
       <c r="C86" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update configuration for stochastic
</commit_message>
<xml_diff>
--- a/spine_rts-gmlc/datasets/branch.xlsx
+++ b/spine_rts-gmlc/datasets/branch.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="branch" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,16 @@
     <sheet name="rel_connection__direction_node" sheetId="3" r:id="rId4"/>
     <sheet name="rel_connection__node__node" sheetId="9" r:id="rId5"/>
     <sheet name="rel_node__commodity" sheetId="5" r:id="rId6"/>
-    <sheet name="rel_node__temporal_block" sheetId="7" r:id="rId7"/>
+    <sheet name="rel__sto_struc__sto_scen" sheetId="11" r:id="rId7"/>
+    <sheet name="rel_node__stochastic_structure" sheetId="10" r:id="rId8"/>
+    <sheet name="rel_node__temporal_block" sheetId="7" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="344">
   <si>
     <t>UID</t>
   </si>
@@ -1036,6 +1038,27 @@
   </si>
   <si>
     <t>energy_carrier</t>
+  </si>
+  <si>
+    <t>stochastic_structure</t>
+  </si>
+  <si>
+    <t>default_none</t>
+  </si>
+  <si>
+    <t>node__stochastic_structure</t>
+  </si>
+  <si>
+    <t>stochastic_scenario</t>
+  </si>
+  <si>
+    <t>stochastic_structure__stochastic_scenario</t>
+  </si>
+  <si>
+    <t>deterministic</t>
+  </si>
+  <si>
+    <t>weight_relative_to_parents</t>
   </si>
 </sst>
 </file>
@@ -12124,8 +12147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection sqref="A1:C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13087,6 +13110,1028 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="36.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D1" t="s">
+        <v>334</v>
+      </c>
+      <c r="E1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C86"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>339</v>
+      </c>
+      <c r="B4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>339</v>
+      </c>
+      <c r="B5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>339</v>
+      </c>
+      <c r="B6" t="s">
+        <v>244</v>
+      </c>
+      <c r="C6" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>339</v>
+      </c>
+      <c r="B7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C7" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>339</v>
+      </c>
+      <c r="B8" t="s">
+        <v>246</v>
+      </c>
+      <c r="C8" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>339</v>
+      </c>
+      <c r="B9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C9" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>339</v>
+      </c>
+      <c r="B10" t="s">
+        <v>248</v>
+      </c>
+      <c r="C10" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>339</v>
+      </c>
+      <c r="B11" t="s">
+        <v>249</v>
+      </c>
+      <c r="C11" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>339</v>
+      </c>
+      <c r="B12" t="s">
+        <v>250</v>
+      </c>
+      <c r="C12" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>339</v>
+      </c>
+      <c r="B13" t="s">
+        <v>251</v>
+      </c>
+      <c r="C13" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>339</v>
+      </c>
+      <c r="B14" t="s">
+        <v>252</v>
+      </c>
+      <c r="C14" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>339</v>
+      </c>
+      <c r="B15" t="s">
+        <v>253</v>
+      </c>
+      <c r="C15" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>339</v>
+      </c>
+      <c r="B16" t="s">
+        <v>254</v>
+      </c>
+      <c r="C16" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>339</v>
+      </c>
+      <c r="B17" t="s">
+        <v>255</v>
+      </c>
+      <c r="C17" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>339</v>
+      </c>
+      <c r="B18" t="s">
+        <v>256</v>
+      </c>
+      <c r="C18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>339</v>
+      </c>
+      <c r="B19" t="s">
+        <v>257</v>
+      </c>
+      <c r="C19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>339</v>
+      </c>
+      <c r="B20" t="s">
+        <v>258</v>
+      </c>
+      <c r="C20" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>339</v>
+      </c>
+      <c r="B21" t="s">
+        <v>259</v>
+      </c>
+      <c r="C21" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>339</v>
+      </c>
+      <c r="B22" t="s">
+        <v>260</v>
+      </c>
+      <c r="C22" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>339</v>
+      </c>
+      <c r="B23" t="s">
+        <v>261</v>
+      </c>
+      <c r="C23" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>339</v>
+      </c>
+      <c r="B24" t="s">
+        <v>262</v>
+      </c>
+      <c r="C24" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>339</v>
+      </c>
+      <c r="B25" t="s">
+        <v>263</v>
+      </c>
+      <c r="C25" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>339</v>
+      </c>
+      <c r="B26" t="s">
+        <v>264</v>
+      </c>
+      <c r="C26" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>339</v>
+      </c>
+      <c r="B27" t="s">
+        <v>265</v>
+      </c>
+      <c r="C27" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>339</v>
+      </c>
+      <c r="B28" t="s">
+        <v>266</v>
+      </c>
+      <c r="C28" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>339</v>
+      </c>
+      <c r="B29" t="s">
+        <v>267</v>
+      </c>
+      <c r="C29" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>339</v>
+      </c>
+      <c r="B30" t="s">
+        <v>268</v>
+      </c>
+      <c r="C30" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>339</v>
+      </c>
+      <c r="B31" t="s">
+        <v>269</v>
+      </c>
+      <c r="C31" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>339</v>
+      </c>
+      <c r="B32" t="s">
+        <v>270</v>
+      </c>
+      <c r="C32" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>339</v>
+      </c>
+      <c r="B33" t="s">
+        <v>271</v>
+      </c>
+      <c r="C33" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>339</v>
+      </c>
+      <c r="B34" t="s">
+        <v>272</v>
+      </c>
+      <c r="C34" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>339</v>
+      </c>
+      <c r="B35" t="s">
+        <v>273</v>
+      </c>
+      <c r="C35" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>339</v>
+      </c>
+      <c r="B36" t="s">
+        <v>274</v>
+      </c>
+      <c r="C36" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>339</v>
+      </c>
+      <c r="B37" t="s">
+        <v>275</v>
+      </c>
+      <c r="C37" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>339</v>
+      </c>
+      <c r="B38" t="s">
+        <v>276</v>
+      </c>
+      <c r="C38" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>339</v>
+      </c>
+      <c r="B39" t="s">
+        <v>277</v>
+      </c>
+      <c r="C39" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>339</v>
+      </c>
+      <c r="B40" t="s">
+        <v>278</v>
+      </c>
+      <c r="C40" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>339</v>
+      </c>
+      <c r="B41" t="s">
+        <v>279</v>
+      </c>
+      <c r="C41" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>339</v>
+      </c>
+      <c r="B42" t="s">
+        <v>280</v>
+      </c>
+      <c r="C42" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>339</v>
+      </c>
+      <c r="B43" t="s">
+        <v>281</v>
+      </c>
+      <c r="C43" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>339</v>
+      </c>
+      <c r="B44" t="s">
+        <v>282</v>
+      </c>
+      <c r="C44" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>339</v>
+      </c>
+      <c r="B45" t="s">
+        <v>283</v>
+      </c>
+      <c r="C45" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>339</v>
+      </c>
+      <c r="B46" t="s">
+        <v>284</v>
+      </c>
+      <c r="C46" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>339</v>
+      </c>
+      <c r="B47" t="s">
+        <v>285</v>
+      </c>
+      <c r="C47" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>339</v>
+      </c>
+      <c r="B48" t="s">
+        <v>286</v>
+      </c>
+      <c r="C48" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>339</v>
+      </c>
+      <c r="B49" t="s">
+        <v>287</v>
+      </c>
+      <c r="C49" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>339</v>
+      </c>
+      <c r="B50" t="s">
+        <v>288</v>
+      </c>
+      <c r="C50" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>339</v>
+      </c>
+      <c r="B51" t="s">
+        <v>289</v>
+      </c>
+      <c r="C51" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>339</v>
+      </c>
+      <c r="B52" t="s">
+        <v>290</v>
+      </c>
+      <c r="C52" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>339</v>
+      </c>
+      <c r="B53" t="s">
+        <v>291</v>
+      </c>
+      <c r="C53" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>339</v>
+      </c>
+      <c r="B54" t="s">
+        <v>292</v>
+      </c>
+      <c r="C54" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>339</v>
+      </c>
+      <c r="B55" t="s">
+        <v>293</v>
+      </c>
+      <c r="C55" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>339</v>
+      </c>
+      <c r="B56" t="s">
+        <v>294</v>
+      </c>
+      <c r="C56" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>339</v>
+      </c>
+      <c r="B57" t="s">
+        <v>295</v>
+      </c>
+      <c r="C57" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>339</v>
+      </c>
+      <c r="B58" t="s">
+        <v>296</v>
+      </c>
+      <c r="C58" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>339</v>
+      </c>
+      <c r="B59" t="s">
+        <v>297</v>
+      </c>
+      <c r="C59" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>339</v>
+      </c>
+      <c r="B60" t="s">
+        <v>298</v>
+      </c>
+      <c r="C60" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>339</v>
+      </c>
+      <c r="B61" t="s">
+        <v>299</v>
+      </c>
+      <c r="C61" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>339</v>
+      </c>
+      <c r="B62" t="s">
+        <v>300</v>
+      </c>
+      <c r="C62" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>339</v>
+      </c>
+      <c r="B63" t="s">
+        <v>301</v>
+      </c>
+      <c r="C63" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>339</v>
+      </c>
+      <c r="B64" t="s">
+        <v>302</v>
+      </c>
+      <c r="C64" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>339</v>
+      </c>
+      <c r="B65" t="s">
+        <v>303</v>
+      </c>
+      <c r="C65" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>339</v>
+      </c>
+      <c r="B66" t="s">
+        <v>304</v>
+      </c>
+      <c r="C66" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>339</v>
+      </c>
+      <c r="B67" t="s">
+        <v>305</v>
+      </c>
+      <c r="C67" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>339</v>
+      </c>
+      <c r="B68" t="s">
+        <v>306</v>
+      </c>
+      <c r="C68" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>339</v>
+      </c>
+      <c r="B69" t="s">
+        <v>307</v>
+      </c>
+      <c r="C69" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>339</v>
+      </c>
+      <c r="B70" t="s">
+        <v>308</v>
+      </c>
+      <c r="C70" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>339</v>
+      </c>
+      <c r="B71" t="s">
+        <v>309</v>
+      </c>
+      <c r="C71" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>339</v>
+      </c>
+      <c r="B72" t="s">
+        <v>310</v>
+      </c>
+      <c r="C72" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>339</v>
+      </c>
+      <c r="B73" t="s">
+        <v>311</v>
+      </c>
+      <c r="C73" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>339</v>
+      </c>
+      <c r="B74" t="s">
+        <v>312</v>
+      </c>
+      <c r="C74" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>339</v>
+      </c>
+      <c r="B75" t="s">
+        <v>313</v>
+      </c>
+      <c r="C75" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>339</v>
+      </c>
+      <c r="B76" t="s">
+        <v>314</v>
+      </c>
+      <c r="C76" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>339</v>
+      </c>
+      <c r="B77" t="s">
+        <v>315</v>
+      </c>
+      <c r="C77" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>339</v>
+      </c>
+      <c r="B78" t="s">
+        <v>316</v>
+      </c>
+      <c r="C78" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>339</v>
+      </c>
+      <c r="B79" t="s">
+        <v>317</v>
+      </c>
+      <c r="C79" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>339</v>
+      </c>
+      <c r="B80" t="s">
+        <v>318</v>
+      </c>
+      <c r="C80" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>339</v>
+      </c>
+      <c r="B81" t="s">
+        <v>319</v>
+      </c>
+      <c r="C81" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>339</v>
+      </c>
+      <c r="B82" t="s">
+        <v>320</v>
+      </c>
+      <c r="C82" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>339</v>
+      </c>
+      <c r="B83" t="s">
+        <v>321</v>
+      </c>
+      <c r="C83" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>339</v>
+      </c>
+      <c r="B84" t="s">
+        <v>322</v>
+      </c>
+      <c r="C84" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>339</v>
+      </c>
+      <c r="B85" t="s">
+        <v>323</v>
+      </c>
+      <c r="C85" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>339</v>
+      </c>
+      <c r="B86" t="s">
+        <v>324</v>
+      </c>
+      <c r="C86" t="s">
+        <v>338</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C171"/>
   <sheetViews>

</xml_diff>

<commit_message>
extend the linear piecewise heat rates to the bus detailed model
</commit_message>
<xml_diff>
--- a/spine_rts-gmlc/datasets/branch.xlsx
+++ b/spine_rts-gmlc/datasets/branch.xlsx
@@ -12182,7 +12182,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12238,7 +12238,7 @@
   <dimension ref="A1:K88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E8:E9"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
modelling CO2 emissions and relevant emission tax
</commit_message>
<xml_diff>
--- a/spine_rts-gmlc/datasets/branch.xlsx
+++ b/spine_rts-gmlc/datasets/branch.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="branch" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1191" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="358">
   <si>
     <t>UID</t>
   </si>
@@ -1093,6 +1093,12 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>Emission_CO2_sink</t>
+  </si>
+  <si>
+    <t>emission_CO2</t>
   </si>
 </sst>
 </file>
@@ -7744,7 +7750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -12235,10 +12241,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K88"/>
+  <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12324,10 +12330,10 @@
         <v>243</v>
       </c>
       <c r="D3" t="s">
-        <v>344</v>
+        <v>356</v>
       </c>
       <c r="E3" t="s">
-        <v>336</v>
+        <v>357</v>
       </c>
       <c r="F3" t="s">
         <v>343</v>
@@ -12350,7 +12356,7 @@
         <v>243</v>
       </c>
       <c r="D4" t="s">
-        <v>332</v>
+        <v>344</v>
       </c>
       <c r="E4" t="s">
         <v>336</v>
@@ -12376,10 +12382,10 @@
         <v>243</v>
       </c>
       <c r="D5" t="s">
-        <v>141</v>
+        <v>332</v>
       </c>
       <c r="E5" t="s">
-        <v>241</v>
+        <v>336</v>
       </c>
       <c r="F5" t="s">
         <v>343</v>
@@ -12402,7 +12408,7 @@
         <v>243</v>
       </c>
       <c r="D6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E6" t="s">
         <v>241</v>
@@ -12428,7 +12434,7 @@
         <v>243</v>
       </c>
       <c r="D7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E7" t="s">
         <v>241</v>
@@ -12454,10 +12460,10 @@
         <v>243</v>
       </c>
       <c r="D8" t="s">
-        <v>244</v>
+        <v>143</v>
       </c>
       <c r="E8" t="s">
-        <v>336</v>
+        <v>241</v>
       </c>
       <c r="F8" t="s">
         <v>343</v>
@@ -12480,7 +12486,7 @@
         <v>243</v>
       </c>
       <c r="D9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E9" t="s">
         <v>336</v>
@@ -12506,7 +12512,7 @@
         <v>243</v>
       </c>
       <c r="D10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E10" t="s">
         <v>336</v>
@@ -12532,7 +12538,7 @@
         <v>243</v>
       </c>
       <c r="D11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E11" t="s">
         <v>336</v>
@@ -12558,7 +12564,7 @@
         <v>243</v>
       </c>
       <c r="D12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E12" t="s">
         <v>336</v>
@@ -12584,7 +12590,7 @@
         <v>243</v>
       </c>
       <c r="D13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E13" t="s">
         <v>336</v>
@@ -12610,7 +12616,7 @@
         <v>243</v>
       </c>
       <c r="D14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E14" t="s">
         <v>336</v>
@@ -12636,7 +12642,7 @@
         <v>243</v>
       </c>
       <c r="D15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E15" t="s">
         <v>336</v>
@@ -12662,7 +12668,7 @@
         <v>243</v>
       </c>
       <c r="D16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E16" t="s">
         <v>336</v>
@@ -12688,7 +12694,7 @@
         <v>243</v>
       </c>
       <c r="D17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E17" t="s">
         <v>336</v>
@@ -12714,7 +12720,7 @@
         <v>243</v>
       </c>
       <c r="D18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E18" t="s">
         <v>336</v>
@@ -12740,7 +12746,7 @@
         <v>243</v>
       </c>
       <c r="D19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E19" t="s">
         <v>336</v>
@@ -12766,7 +12772,7 @@
         <v>243</v>
       </c>
       <c r="D20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E20" t="s">
         <v>336</v>
@@ -12792,7 +12798,7 @@
         <v>243</v>
       </c>
       <c r="D21" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E21" t="s">
         <v>336</v>
@@ -12818,7 +12824,7 @@
         <v>243</v>
       </c>
       <c r="D22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E22" t="s">
         <v>336</v>
@@ -12844,7 +12850,7 @@
         <v>243</v>
       </c>
       <c r="D23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E23" t="s">
         <v>336</v>
@@ -12870,7 +12876,7 @@
         <v>243</v>
       </c>
       <c r="D24" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E24" t="s">
         <v>336</v>
@@ -12896,7 +12902,7 @@
         <v>243</v>
       </c>
       <c r="D25" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E25" t="s">
         <v>336</v>
@@ -12922,7 +12928,7 @@
         <v>243</v>
       </c>
       <c r="D26" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E26" t="s">
         <v>336</v>
@@ -12948,7 +12954,7 @@
         <v>243</v>
       </c>
       <c r="D27" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E27" t="s">
         <v>336</v>
@@ -12974,7 +12980,7 @@
         <v>243</v>
       </c>
       <c r="D28" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E28" t="s">
         <v>336</v>
@@ -13000,7 +13006,7 @@
         <v>243</v>
       </c>
       <c r="D29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E29" t="s">
         <v>336</v>
@@ -13026,7 +13032,7 @@
         <v>243</v>
       </c>
       <c r="D30" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E30" t="s">
         <v>336</v>
@@ -13052,7 +13058,7 @@
         <v>243</v>
       </c>
       <c r="D31" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E31" t="s">
         <v>336</v>
@@ -13078,7 +13084,7 @@
         <v>243</v>
       </c>
       <c r="D32" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E32" t="s">
         <v>336</v>
@@ -13104,7 +13110,7 @@
         <v>243</v>
       </c>
       <c r="D33" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E33" t="s">
         <v>336</v>
@@ -13130,7 +13136,7 @@
         <v>243</v>
       </c>
       <c r="D34" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E34" t="s">
         <v>336</v>
@@ -13156,7 +13162,7 @@
         <v>243</v>
       </c>
       <c r="D35" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E35" t="s">
         <v>336</v>
@@ -13182,7 +13188,7 @@
         <v>243</v>
       </c>
       <c r="D36" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E36" t="s">
         <v>336</v>
@@ -13208,7 +13214,7 @@
         <v>243</v>
       </c>
       <c r="D37" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E37" t="s">
         <v>336</v>
@@ -13234,7 +13240,7 @@
         <v>243</v>
       </c>
       <c r="D38" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E38" t="s">
         <v>336</v>
@@ -13260,7 +13266,7 @@
         <v>243</v>
       </c>
       <c r="D39" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E39" t="s">
         <v>336</v>
@@ -13286,7 +13292,7 @@
         <v>243</v>
       </c>
       <c r="D40" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E40" t="s">
         <v>336</v>
@@ -13312,7 +13318,7 @@
         <v>243</v>
       </c>
       <c r="D41" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E41" t="s">
         <v>336</v>
@@ -13338,7 +13344,7 @@
         <v>243</v>
       </c>
       <c r="D42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E42" t="s">
         <v>336</v>
@@ -13364,7 +13370,7 @@
         <v>243</v>
       </c>
       <c r="D43" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E43" t="s">
         <v>336</v>
@@ -13390,7 +13396,7 @@
         <v>243</v>
       </c>
       <c r="D44" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E44" t="s">
         <v>336</v>
@@ -13416,7 +13422,7 @@
         <v>243</v>
       </c>
       <c r="D45" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E45" t="s">
         <v>336</v>
@@ -13442,7 +13448,7 @@
         <v>243</v>
       </c>
       <c r="D46" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E46" t="s">
         <v>336</v>
@@ -13468,7 +13474,7 @@
         <v>243</v>
       </c>
       <c r="D47" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E47" t="s">
         <v>336</v>
@@ -13494,7 +13500,7 @@
         <v>243</v>
       </c>
       <c r="D48" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E48" t="s">
         <v>336</v>
@@ -13520,7 +13526,7 @@
         <v>243</v>
       </c>
       <c r="D49" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E49" t="s">
         <v>336</v>
@@ -13546,7 +13552,7 @@
         <v>243</v>
       </c>
       <c r="D50" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E50" t="s">
         <v>336</v>
@@ -13572,7 +13578,7 @@
         <v>243</v>
       </c>
       <c r="D51" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E51" t="s">
         <v>336</v>
@@ -13598,7 +13604,7 @@
         <v>243</v>
       </c>
       <c r="D52" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E52" t="s">
         <v>336</v>
@@ -13624,7 +13630,7 @@
         <v>243</v>
       </c>
       <c r="D53" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E53" t="s">
         <v>336</v>
@@ -13650,7 +13656,7 @@
         <v>243</v>
       </c>
       <c r="D54" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E54" t="s">
         <v>336</v>
@@ -13676,7 +13682,7 @@
         <v>243</v>
       </c>
       <c r="D55" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E55" t="s">
         <v>336</v>
@@ -13702,7 +13708,7 @@
         <v>243</v>
       </c>
       <c r="D56" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E56" t="s">
         <v>336</v>
@@ -13728,7 +13734,7 @@
         <v>243</v>
       </c>
       <c r="D57" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E57" t="s">
         <v>336</v>
@@ -13754,7 +13760,7 @@
         <v>243</v>
       </c>
       <c r="D58" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E58" t="s">
         <v>336</v>
@@ -13780,7 +13786,7 @@
         <v>243</v>
       </c>
       <c r="D59" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E59" t="s">
         <v>336</v>
@@ -13806,7 +13812,7 @@
         <v>243</v>
       </c>
       <c r="D60" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E60" t="s">
         <v>336</v>
@@ -13832,7 +13838,7 @@
         <v>243</v>
       </c>
       <c r="D61" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E61" t="s">
         <v>336</v>
@@ -13858,7 +13864,7 @@
         <v>243</v>
       </c>
       <c r="D62" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E62" t="s">
         <v>336</v>
@@ -13884,7 +13890,7 @@
         <v>243</v>
       </c>
       <c r="D63" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E63" t="s">
         <v>336</v>
@@ -13910,7 +13916,7 @@
         <v>243</v>
       </c>
       <c r="D64" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E64" t="s">
         <v>336</v>
@@ -13936,7 +13942,7 @@
         <v>243</v>
       </c>
       <c r="D65" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E65" t="s">
         <v>336</v>
@@ -13962,7 +13968,7 @@
         <v>243</v>
       </c>
       <c r="D66" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E66" t="s">
         <v>336</v>
@@ -13988,7 +13994,7 @@
         <v>243</v>
       </c>
       <c r="D67" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E67" t="s">
         <v>336</v>
@@ -14014,7 +14020,7 @@
         <v>243</v>
       </c>
       <c r="D68" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E68" t="s">
         <v>336</v>
@@ -14040,7 +14046,7 @@
         <v>243</v>
       </c>
       <c r="D69" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E69" t="s">
         <v>336</v>
@@ -14066,7 +14072,7 @@
         <v>243</v>
       </c>
       <c r="D70" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E70" t="s">
         <v>336</v>
@@ -14092,7 +14098,7 @@
         <v>243</v>
       </c>
       <c r="D71" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E71" t="s">
         <v>336</v>
@@ -14118,7 +14124,7 @@
         <v>243</v>
       </c>
       <c r="D72" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E72" t="s">
         <v>336</v>
@@ -14144,7 +14150,7 @@
         <v>243</v>
       </c>
       <c r="D73" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E73" t="s">
         <v>336</v>
@@ -14170,7 +14176,7 @@
         <v>243</v>
       </c>
       <c r="D74" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E74" t="s">
         <v>336</v>
@@ -14196,7 +14202,7 @@
         <v>243</v>
       </c>
       <c r="D75" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E75" t="s">
         <v>336</v>
@@ -14222,7 +14228,7 @@
         <v>243</v>
       </c>
       <c r="D76" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E76" t="s">
         <v>336</v>
@@ -14248,7 +14254,7 @@
         <v>243</v>
       </c>
       <c r="D77" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E77" t="s">
         <v>336</v>
@@ -14274,7 +14280,7 @@
         <v>243</v>
       </c>
       <c r="D78" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E78" t="s">
         <v>336</v>
@@ -14300,7 +14306,7 @@
         <v>243</v>
       </c>
       <c r="D79" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E79" t="s">
         <v>336</v>
@@ -14326,7 +14332,7 @@
         <v>243</v>
       </c>
       <c r="D80" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E80" t="s">
         <v>336</v>
@@ -14352,7 +14358,7 @@
         <v>243</v>
       </c>
       <c r="D81" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E81" t="s">
         <v>336</v>
@@ -14378,7 +14384,7 @@
         <v>243</v>
       </c>
       <c r="D82" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E82" t="s">
         <v>336</v>
@@ -14404,7 +14410,7 @@
         <v>243</v>
       </c>
       <c r="D83" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E83" t="s">
         <v>336</v>
@@ -14430,7 +14436,7 @@
         <v>243</v>
       </c>
       <c r="D84" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E84" t="s">
         <v>336</v>
@@ -14456,7 +14462,7 @@
         <v>243</v>
       </c>
       <c r="D85" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E85" t="s">
         <v>336</v>
@@ -14482,7 +14488,7 @@
         <v>243</v>
       </c>
       <c r="D86" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E86" t="s">
         <v>336</v>
@@ -14508,7 +14514,7 @@
         <v>243</v>
       </c>
       <c r="D87" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E87" t="s">
         <v>336</v>
@@ -14534,7 +14540,7 @@
         <v>243</v>
       </c>
       <c r="D88" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E88" t="s">
         <v>336</v>
@@ -14546,6 +14552,32 @@
         <v>326</v>
       </c>
       <c r="H88" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>240</v>
+      </c>
+      <c r="B89" t="s">
+        <v>338</v>
+      </c>
+      <c r="C89" t="s">
+        <v>243</v>
+      </c>
+      <c r="D89" t="s">
+        <v>324</v>
+      </c>
+      <c r="E89" t="s">
+        <v>336</v>
+      </c>
+      <c r="F89" t="s">
+        <v>343</v>
+      </c>
+      <c r="G89" t="s">
+        <v>326</v>
+      </c>
+      <c r="H89" t="s">
         <v>327</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update system structure with respect to new changes
</commit_message>
<xml_diff>
--- a/spine_rts-gmlc/datasets/branch.xlsx
+++ b/spine_rts-gmlc/datasets/branch.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="branch" sheetId="1" r:id="rId1"/>
@@ -1005,12 +1005,6 @@
     <t>connection__node__node</t>
   </si>
   <si>
-    <t>blk_t1</t>
-  </si>
-  <si>
-    <t>blk_t2</t>
-  </si>
-  <si>
     <t>connection_capacity</t>
   </si>
   <si>
@@ -1099,6 +1093,12 @@
   </si>
   <si>
     <t>emission_CO2</t>
+  </si>
+  <si>
+    <t>tb1_core</t>
+  </si>
+  <si>
+    <t>tb2_look_ahead</t>
   </si>
 </sst>
 </file>
@@ -7750,7 +7750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -11314,7 +11314,7 @@
         <v>135</v>
       </c>
       <c r="B7" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -11355,24 +11355,24 @@
         <v>136</v>
       </c>
       <c r="D1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C2" t="s">
         <v>141</v>
       </c>
       <c r="D2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -11380,16 +11380,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>331</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>333</v>
       </c>
       <c r="C3" t="s">
         <v>141</v>
       </c>
       <c r="D3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E3">
         <v>100</v>
@@ -11398,16 +11398,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C4" t="s">
         <v>143</v>
       </c>
       <c r="D4" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -11416,16 +11416,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>331</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>333</v>
       </c>
       <c r="C5" t="s">
         <v>143</v>
       </c>
       <c r="D5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E5">
         <v>100</v>
@@ -11434,7 +11434,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>236</v>
@@ -11443,7 +11443,7 @@
         <v>141</v>
       </c>
       <c r="D6" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E6">
         <v>175</v>
@@ -11451,7 +11451,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>236</v>
@@ -11460,7 +11460,7 @@
         <v>141</v>
       </c>
       <c r="D7" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E7">
         <v>175</v>
@@ -11468,7 +11468,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>236</v>
@@ -11477,7 +11477,7 @@
         <v>142</v>
       </c>
       <c r="D8" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E8">
         <v>175</v>
@@ -11485,7 +11485,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>236</v>
@@ -11494,7 +11494,7 @@
         <v>142</v>
       </c>
       <c r="D9" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E9">
         <v>175</v>
@@ -11502,7 +11502,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>237</v>
@@ -11511,7 +11511,7 @@
         <v>141</v>
       </c>
       <c r="D10" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E10">
         <v>500</v>
@@ -11519,7 +11519,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>237</v>
@@ -11528,7 +11528,7 @@
         <v>141</v>
       </c>
       <c r="D11" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E11">
         <v>500</v>
@@ -11536,7 +11536,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>237</v>
@@ -11545,7 +11545,7 @@
         <v>142</v>
       </c>
       <c r="D12" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E12">
         <v>500</v>
@@ -11553,7 +11553,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>237</v>
@@ -11562,7 +11562,7 @@
         <v>142</v>
       </c>
       <c r="D13" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E13">
         <v>500</v>
@@ -11570,7 +11570,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>238</v>
@@ -11579,7 +11579,7 @@
         <v>141</v>
       </c>
       <c r="D14" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E14">
         <v>500</v>
@@ -11587,7 +11587,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>238</v>
@@ -11596,7 +11596,7 @@
         <v>141</v>
       </c>
       <c r="D15" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E15">
         <v>500</v>
@@ -11604,7 +11604,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>238</v>
@@ -11613,7 +11613,7 @@
         <v>142</v>
       </c>
       <c r="D16" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E16">
         <v>500</v>
@@ -11621,7 +11621,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>238</v>
@@ -11630,7 +11630,7 @@
         <v>142</v>
       </c>
       <c r="D17" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E17">
         <v>500</v>
@@ -11638,7 +11638,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>139</v>
@@ -11647,7 +11647,7 @@
         <v>141</v>
       </c>
       <c r="D18" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E18">
         <v>500</v>
@@ -11655,7 +11655,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>139</v>
@@ -11664,7 +11664,7 @@
         <v>141</v>
       </c>
       <c r="D19" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E19">
         <v>500</v>
@@ -11672,7 +11672,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>139</v>
@@ -11681,7 +11681,7 @@
         <v>143</v>
       </c>
       <c r="D20" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E20">
         <v>500</v>
@@ -11689,7 +11689,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>139</v>
@@ -11698,7 +11698,7 @@
         <v>143</v>
       </c>
       <c r="D21" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E21">
         <v>500</v>
@@ -11706,7 +11706,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>140</v>
@@ -11715,7 +11715,7 @@
         <v>142</v>
       </c>
       <c r="D22" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E22">
         <v>500</v>
@@ -11723,7 +11723,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>140</v>
@@ -11732,7 +11732,7 @@
         <v>142</v>
       </c>
       <c r="D23" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E23">
         <v>500</v>
@@ -11740,7 +11740,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>140</v>
@@ -11749,7 +11749,7 @@
         <v>143</v>
       </c>
       <c r="D24" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E24">
         <v>500</v>
@@ -11757,7 +11757,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>140</v>
@@ -11766,7 +11766,7 @@
         <v>143</v>
       </c>
       <c r="D25" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E25">
         <v>500</v>
@@ -11875,10 +11875,10 @@
         <v>136</v>
       </c>
       <c r="E1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -11895,7 +11895,7 @@
         <v>142</v>
       </c>
       <c r="E2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F2">
         <v>0.99</v>
@@ -11915,7 +11915,7 @@
         <v>142</v>
       </c>
       <c r="E3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F3">
         <v>0.99</v>
@@ -11935,7 +11935,7 @@
         <v>142</v>
       </c>
       <c r="E4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F4">
         <v>0.99</v>
@@ -11955,7 +11955,7 @@
         <v>143</v>
       </c>
       <c r="E5" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F5">
         <v>0.99</v>
@@ -11975,7 +11975,7 @@
         <v>143</v>
       </c>
       <c r="E6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F6">
         <v>0.99</v>
@@ -11995,7 +11995,7 @@
         <v>141</v>
       </c>
       <c r="E7" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F7">
         <v>0.99</v>
@@ -12015,7 +12015,7 @@
         <v>141</v>
       </c>
       <c r="E8" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F8">
         <v>0.99</v>
@@ -12035,7 +12035,7 @@
         <v>141</v>
       </c>
       <c r="E9" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F9">
         <v>0.99</v>
@@ -12055,7 +12055,7 @@
         <v>141</v>
       </c>
       <c r="E10" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F10">
         <v>0.99</v>
@@ -12075,7 +12075,7 @@
         <v>142</v>
       </c>
       <c r="E11" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F11">
         <v>0.99</v>
@@ -12086,7 +12086,7 @@
         <v>325</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C12" t="s">
         <v>141</v>
@@ -12095,7 +12095,7 @@
         <v>143</v>
       </c>
       <c r="E12" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F12">
         <v>0.99</v>
@@ -12106,7 +12106,7 @@
         <v>325</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C13" t="s">
         <v>143</v>
@@ -12115,7 +12115,7 @@
         <v>141</v>
       </c>
       <c r="E13" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F13">
         <v>0.99</v>
@@ -12205,30 +12205,30 @@
         <v>134</v>
       </c>
       <c r="B1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C1" t="s">
         <v>337</v>
       </c>
-      <c r="C1" t="s">
-        <v>339</v>
-      </c>
       <c r="D1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C2" t="s">
+        <v>339</v>
+      </c>
+      <c r="D2" t="s">
         <v>340</v>
-      </c>
-      <c r="B2" t="s">
-        <v>343</v>
-      </c>
-      <c r="C2" t="s">
-        <v>341</v>
-      </c>
-      <c r="D2" t="s">
-        <v>342</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -12243,8 +12243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12266,36 +12266,36 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="J1" t="s">
+        <v>347</v>
+      </c>
+      <c r="K1" t="s">
         <v>348</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="J1" t="s">
-        <v>349</v>
-      </c>
-      <c r="K1" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>343</v>
+      </c>
+      <c r="B2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C2" t="s">
         <v>345</v>
-      </c>
-      <c r="B2" t="s">
-        <v>346</v>
-      </c>
-      <c r="C2" t="s">
-        <v>347</v>
       </c>
       <c r="D2" t="s">
         <v>136</v>
@@ -12304,7 +12304,7 @@
         <v>239</v>
       </c>
       <c r="F2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G2" t="s">
         <v>242</v>
@@ -12313,10 +12313,10 @@
         <v>242</v>
       </c>
       <c r="J2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="K2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -12324,25 +12324,25 @@
         <v>240</v>
       </c>
       <c r="B3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C3" t="s">
         <v>243</v>
       </c>
       <c r="D3" t="s">
+        <v>354</v>
+      </c>
+      <c r="E3" t="s">
+        <v>355</v>
+      </c>
+      <c r="F3" t="s">
+        <v>341</v>
+      </c>
+      <c r="G3" t="s">
         <v>356</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>357</v>
-      </c>
-      <c r="F3" t="s">
-        <v>343</v>
-      </c>
-      <c r="G3" t="s">
-        <v>326</v>
-      </c>
-      <c r="H3" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -12350,25 +12350,25 @@
         <v>240</v>
       </c>
       <c r="B4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C4" t="s">
         <v>243</v>
       </c>
       <c r="D4" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F4" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G4" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H4" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -12376,25 +12376,25 @@
         <v>240</v>
       </c>
       <c r="B5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C5" t="s">
         <v>243</v>
       </c>
       <c r="D5" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E5" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F5" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G5" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H5" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -12402,7 +12402,7 @@
         <v>240</v>
       </c>
       <c r="B6" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C6" t="s">
         <v>243</v>
@@ -12414,13 +12414,13 @@
         <v>241</v>
       </c>
       <c r="F6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G6" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H6" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -12428,7 +12428,7 @@
         <v>240</v>
       </c>
       <c r="B7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C7" t="s">
         <v>243</v>
@@ -12440,13 +12440,13 @@
         <v>241</v>
       </c>
       <c r="F7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G7" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H7" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -12454,7 +12454,7 @@
         <v>240</v>
       </c>
       <c r="B8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C8" t="s">
         <v>243</v>
@@ -12466,13 +12466,13 @@
         <v>241</v>
       </c>
       <c r="F8" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G8" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H8" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -12480,7 +12480,7 @@
         <v>240</v>
       </c>
       <c r="B9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C9" t="s">
         <v>243</v>
@@ -12489,16 +12489,16 @@
         <v>244</v>
       </c>
       <c r="E9" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F9" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G9" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H9" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -12506,7 +12506,7 @@
         <v>240</v>
       </c>
       <c r="B10" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C10" t="s">
         <v>243</v>
@@ -12515,16 +12515,16 @@
         <v>245</v>
       </c>
       <c r="E10" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G10" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H10" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -12532,7 +12532,7 @@
         <v>240</v>
       </c>
       <c r="B11" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C11" t="s">
         <v>243</v>
@@ -12541,16 +12541,16 @@
         <v>246</v>
       </c>
       <c r="E11" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F11" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G11" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H11" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -12558,7 +12558,7 @@
         <v>240</v>
       </c>
       <c r="B12" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C12" t="s">
         <v>243</v>
@@ -12567,16 +12567,16 @@
         <v>247</v>
       </c>
       <c r="E12" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F12" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G12" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H12" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -12584,7 +12584,7 @@
         <v>240</v>
       </c>
       <c r="B13" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C13" t="s">
         <v>243</v>
@@ -12593,16 +12593,16 @@
         <v>248</v>
       </c>
       <c r="E13" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F13" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G13" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H13" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -12610,7 +12610,7 @@
         <v>240</v>
       </c>
       <c r="B14" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C14" t="s">
         <v>243</v>
@@ -12619,16 +12619,16 @@
         <v>249</v>
       </c>
       <c r="E14" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F14" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G14" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H14" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -12636,7 +12636,7 @@
         <v>240</v>
       </c>
       <c r="B15" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C15" t="s">
         <v>243</v>
@@ -12645,16 +12645,16 @@
         <v>250</v>
       </c>
       <c r="E15" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G15" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H15" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -12662,7 +12662,7 @@
         <v>240</v>
       </c>
       <c r="B16" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C16" t="s">
         <v>243</v>
@@ -12671,16 +12671,16 @@
         <v>251</v>
       </c>
       <c r="E16" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F16" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G16" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H16" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -12688,7 +12688,7 @@
         <v>240</v>
       </c>
       <c r="B17" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C17" t="s">
         <v>243</v>
@@ -12697,16 +12697,16 @@
         <v>252</v>
       </c>
       <c r="E17" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F17" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G17" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H17" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -12714,7 +12714,7 @@
         <v>240</v>
       </c>
       <c r="B18" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C18" t="s">
         <v>243</v>
@@ -12723,16 +12723,16 @@
         <v>253</v>
       </c>
       <c r="E18" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F18" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G18" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H18" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -12740,7 +12740,7 @@
         <v>240</v>
       </c>
       <c r="B19" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C19" t="s">
         <v>243</v>
@@ -12749,16 +12749,16 @@
         <v>254</v>
       </c>
       <c r="E19" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F19" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G19" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H19" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -12766,7 +12766,7 @@
         <v>240</v>
       </c>
       <c r="B20" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C20" t="s">
         <v>243</v>
@@ -12775,16 +12775,16 @@
         <v>255</v>
       </c>
       <c r="E20" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F20" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G20" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H20" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -12792,7 +12792,7 @@
         <v>240</v>
       </c>
       <c r="B21" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C21" t="s">
         <v>243</v>
@@ -12801,16 +12801,16 @@
         <v>256</v>
       </c>
       <c r="E21" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F21" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G21" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H21" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -12818,7 +12818,7 @@
         <v>240</v>
       </c>
       <c r="B22" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C22" t="s">
         <v>243</v>
@@ -12827,16 +12827,16 @@
         <v>257</v>
       </c>
       <c r="E22" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F22" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G22" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H22" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -12844,7 +12844,7 @@
         <v>240</v>
       </c>
       <c r="B23" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C23" t="s">
         <v>243</v>
@@ -12853,16 +12853,16 @@
         <v>258</v>
       </c>
       <c r="E23" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F23" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G23" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H23" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -12870,7 +12870,7 @@
         <v>240</v>
       </c>
       <c r="B24" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C24" t="s">
         <v>243</v>
@@ -12879,16 +12879,16 @@
         <v>259</v>
       </c>
       <c r="E24" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F24" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G24" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H24" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -12896,7 +12896,7 @@
         <v>240</v>
       </c>
       <c r="B25" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C25" t="s">
         <v>243</v>
@@ -12905,16 +12905,16 @@
         <v>260</v>
       </c>
       <c r="E25" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F25" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G25" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H25" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -12922,7 +12922,7 @@
         <v>240</v>
       </c>
       <c r="B26" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C26" t="s">
         <v>243</v>
@@ -12931,16 +12931,16 @@
         <v>261</v>
       </c>
       <c r="E26" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F26" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G26" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H26" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -12948,7 +12948,7 @@
         <v>240</v>
       </c>
       <c r="B27" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C27" t="s">
         <v>243</v>
@@ -12957,16 +12957,16 @@
         <v>262</v>
       </c>
       <c r="E27" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F27" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G27" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H27" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -12974,7 +12974,7 @@
         <v>240</v>
       </c>
       <c r="B28" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C28" t="s">
         <v>243</v>
@@ -12983,16 +12983,16 @@
         <v>263</v>
       </c>
       <c r="E28" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F28" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G28" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H28" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -13000,7 +13000,7 @@
         <v>240</v>
       </c>
       <c r="B29" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C29" t="s">
         <v>243</v>
@@ -13009,16 +13009,16 @@
         <v>264</v>
       </c>
       <c r="E29" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F29" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G29" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H29" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -13026,7 +13026,7 @@
         <v>240</v>
       </c>
       <c r="B30" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C30" t="s">
         <v>243</v>
@@ -13035,16 +13035,16 @@
         <v>265</v>
       </c>
       <c r="E30" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F30" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G30" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H30" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -13052,7 +13052,7 @@
         <v>240</v>
       </c>
       <c r="B31" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C31" t="s">
         <v>243</v>
@@ -13061,16 +13061,16 @@
         <v>266</v>
       </c>
       <c r="E31" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F31" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G31" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H31" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -13078,7 +13078,7 @@
         <v>240</v>
       </c>
       <c r="B32" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C32" t="s">
         <v>243</v>
@@ -13087,16 +13087,16 @@
         <v>267</v>
       </c>
       <c r="E32" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F32" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G32" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H32" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -13104,7 +13104,7 @@
         <v>240</v>
       </c>
       <c r="B33" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C33" t="s">
         <v>243</v>
@@ -13113,16 +13113,16 @@
         <v>268</v>
       </c>
       <c r="E33" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F33" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G33" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H33" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -13130,7 +13130,7 @@
         <v>240</v>
       </c>
       <c r="B34" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C34" t="s">
         <v>243</v>
@@ -13139,16 +13139,16 @@
         <v>269</v>
       </c>
       <c r="E34" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F34" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G34" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H34" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -13156,7 +13156,7 @@
         <v>240</v>
       </c>
       <c r="B35" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C35" t="s">
         <v>243</v>
@@ -13165,16 +13165,16 @@
         <v>270</v>
       </c>
       <c r="E35" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F35" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G35" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H35" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -13182,7 +13182,7 @@
         <v>240</v>
       </c>
       <c r="B36" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C36" t="s">
         <v>243</v>
@@ -13191,16 +13191,16 @@
         <v>271</v>
       </c>
       <c r="E36" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G36" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H36" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -13208,7 +13208,7 @@
         <v>240</v>
       </c>
       <c r="B37" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C37" t="s">
         <v>243</v>
@@ -13217,16 +13217,16 @@
         <v>272</v>
       </c>
       <c r="E37" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F37" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G37" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H37" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -13234,7 +13234,7 @@
         <v>240</v>
       </c>
       <c r="B38" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C38" t="s">
         <v>243</v>
@@ -13243,16 +13243,16 @@
         <v>273</v>
       </c>
       <c r="E38" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F38" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G38" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H38" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -13260,7 +13260,7 @@
         <v>240</v>
       </c>
       <c r="B39" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C39" t="s">
         <v>243</v>
@@ -13269,16 +13269,16 @@
         <v>274</v>
       </c>
       <c r="E39" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F39" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G39" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H39" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -13286,7 +13286,7 @@
         <v>240</v>
       </c>
       <c r="B40" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C40" t="s">
         <v>243</v>
@@ -13295,16 +13295,16 @@
         <v>275</v>
       </c>
       <c r="E40" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F40" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G40" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H40" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -13312,7 +13312,7 @@
         <v>240</v>
       </c>
       <c r="B41" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C41" t="s">
         <v>243</v>
@@ -13321,16 +13321,16 @@
         <v>276</v>
       </c>
       <c r="E41" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F41" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G41" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H41" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -13338,7 +13338,7 @@
         <v>240</v>
       </c>
       <c r="B42" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C42" t="s">
         <v>243</v>
@@ -13347,16 +13347,16 @@
         <v>277</v>
       </c>
       <c r="E42" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F42" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G42" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H42" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -13364,7 +13364,7 @@
         <v>240</v>
       </c>
       <c r="B43" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C43" t="s">
         <v>243</v>
@@ -13373,16 +13373,16 @@
         <v>278</v>
       </c>
       <c r="E43" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F43" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G43" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H43" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -13390,7 +13390,7 @@
         <v>240</v>
       </c>
       <c r="B44" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C44" t="s">
         <v>243</v>
@@ -13399,16 +13399,16 @@
         <v>279</v>
       </c>
       <c r="E44" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F44" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G44" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H44" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -13416,7 +13416,7 @@
         <v>240</v>
       </c>
       <c r="B45" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C45" t="s">
         <v>243</v>
@@ -13425,16 +13425,16 @@
         <v>280</v>
       </c>
       <c r="E45" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F45" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G45" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H45" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -13442,7 +13442,7 @@
         <v>240</v>
       </c>
       <c r="B46" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C46" t="s">
         <v>243</v>
@@ -13451,16 +13451,16 @@
         <v>281</v>
       </c>
       <c r="E46" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F46" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G46" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H46" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -13468,7 +13468,7 @@
         <v>240</v>
       </c>
       <c r="B47" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C47" t="s">
         <v>243</v>
@@ -13477,16 +13477,16 @@
         <v>282</v>
       </c>
       <c r="E47" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F47" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G47" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H47" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -13494,7 +13494,7 @@
         <v>240</v>
       </c>
       <c r="B48" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C48" t="s">
         <v>243</v>
@@ -13503,16 +13503,16 @@
         <v>283</v>
       </c>
       <c r="E48" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F48" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G48" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H48" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -13520,7 +13520,7 @@
         <v>240</v>
       </c>
       <c r="B49" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C49" t="s">
         <v>243</v>
@@ -13529,16 +13529,16 @@
         <v>284</v>
       </c>
       <c r="E49" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F49" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G49" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H49" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -13546,7 +13546,7 @@
         <v>240</v>
       </c>
       <c r="B50" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C50" t="s">
         <v>243</v>
@@ -13555,16 +13555,16 @@
         <v>285</v>
       </c>
       <c r="E50" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F50" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G50" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H50" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -13572,7 +13572,7 @@
         <v>240</v>
       </c>
       <c r="B51" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C51" t="s">
         <v>243</v>
@@ -13581,16 +13581,16 @@
         <v>286</v>
       </c>
       <c r="E51" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F51" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G51" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H51" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -13598,7 +13598,7 @@
         <v>240</v>
       </c>
       <c r="B52" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C52" t="s">
         <v>243</v>
@@ -13607,16 +13607,16 @@
         <v>287</v>
       </c>
       <c r="E52" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F52" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G52" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H52" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -13624,7 +13624,7 @@
         <v>240</v>
       </c>
       <c r="B53" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C53" t="s">
         <v>243</v>
@@ -13633,16 +13633,16 @@
         <v>288</v>
       </c>
       <c r="E53" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F53" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G53" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H53" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -13650,7 +13650,7 @@
         <v>240</v>
       </c>
       <c r="B54" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C54" t="s">
         <v>243</v>
@@ -13659,16 +13659,16 @@
         <v>289</v>
       </c>
       <c r="E54" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F54" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G54" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H54" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -13676,7 +13676,7 @@
         <v>240</v>
       </c>
       <c r="B55" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C55" t="s">
         <v>243</v>
@@ -13685,16 +13685,16 @@
         <v>290</v>
       </c>
       <c r="E55" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F55" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G55" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H55" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -13702,7 +13702,7 @@
         <v>240</v>
       </c>
       <c r="B56" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C56" t="s">
         <v>243</v>
@@ -13711,16 +13711,16 @@
         <v>291</v>
       </c>
       <c r="E56" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F56" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G56" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H56" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -13728,7 +13728,7 @@
         <v>240</v>
       </c>
       <c r="B57" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C57" t="s">
         <v>243</v>
@@ -13737,16 +13737,16 @@
         <v>292</v>
       </c>
       <c r="E57" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F57" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G57" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H57" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -13754,7 +13754,7 @@
         <v>240</v>
       </c>
       <c r="B58" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C58" t="s">
         <v>243</v>
@@ -13763,16 +13763,16 @@
         <v>293</v>
       </c>
       <c r="E58" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F58" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G58" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H58" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -13780,7 +13780,7 @@
         <v>240</v>
       </c>
       <c r="B59" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C59" t="s">
         <v>243</v>
@@ -13789,16 +13789,16 @@
         <v>294</v>
       </c>
       <c r="E59" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F59" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G59" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H59" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -13806,7 +13806,7 @@
         <v>240</v>
       </c>
       <c r="B60" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C60" t="s">
         <v>243</v>
@@ -13815,16 +13815,16 @@
         <v>295</v>
       </c>
       <c r="E60" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F60" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G60" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H60" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -13832,7 +13832,7 @@
         <v>240</v>
       </c>
       <c r="B61" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C61" t="s">
         <v>243</v>
@@ -13841,16 +13841,16 @@
         <v>296</v>
       </c>
       <c r="E61" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F61" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G61" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H61" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -13858,7 +13858,7 @@
         <v>240</v>
       </c>
       <c r="B62" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C62" t="s">
         <v>243</v>
@@ -13867,16 +13867,16 @@
         <v>297</v>
       </c>
       <c r="E62" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F62" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G62" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H62" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -13884,7 +13884,7 @@
         <v>240</v>
       </c>
       <c r="B63" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C63" t="s">
         <v>243</v>
@@ -13893,16 +13893,16 @@
         <v>298</v>
       </c>
       <c r="E63" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F63" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G63" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H63" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -13910,7 +13910,7 @@
         <v>240</v>
       </c>
       <c r="B64" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C64" t="s">
         <v>243</v>
@@ -13919,16 +13919,16 @@
         <v>299</v>
       </c>
       <c r="E64" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F64" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G64" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H64" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -13936,7 +13936,7 @@
         <v>240</v>
       </c>
       <c r="B65" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C65" t="s">
         <v>243</v>
@@ -13945,16 +13945,16 @@
         <v>300</v>
       </c>
       <c r="E65" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F65" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G65" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H65" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -13962,7 +13962,7 @@
         <v>240</v>
       </c>
       <c r="B66" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C66" t="s">
         <v>243</v>
@@ -13971,16 +13971,16 @@
         <v>301</v>
       </c>
       <c r="E66" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F66" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G66" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H66" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -13988,7 +13988,7 @@
         <v>240</v>
       </c>
       <c r="B67" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C67" t="s">
         <v>243</v>
@@ -13997,16 +13997,16 @@
         <v>302</v>
       </c>
       <c r="E67" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F67" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G67" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H67" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -14014,7 +14014,7 @@
         <v>240</v>
       </c>
       <c r="B68" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C68" t="s">
         <v>243</v>
@@ -14023,16 +14023,16 @@
         <v>303</v>
       </c>
       <c r="E68" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F68" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G68" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H68" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -14040,7 +14040,7 @@
         <v>240</v>
       </c>
       <c r="B69" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C69" t="s">
         <v>243</v>
@@ -14049,16 +14049,16 @@
         <v>304</v>
       </c>
       <c r="E69" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F69" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G69" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H69" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -14066,7 +14066,7 @@
         <v>240</v>
       </c>
       <c r="B70" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C70" t="s">
         <v>243</v>
@@ -14075,16 +14075,16 @@
         <v>305</v>
       </c>
       <c r="E70" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F70" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G70" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H70" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -14092,7 +14092,7 @@
         <v>240</v>
       </c>
       <c r="B71" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C71" t="s">
         <v>243</v>
@@ -14101,16 +14101,16 @@
         <v>306</v>
       </c>
       <c r="E71" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F71" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G71" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H71" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -14118,7 +14118,7 @@
         <v>240</v>
       </c>
       <c r="B72" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C72" t="s">
         <v>243</v>
@@ -14127,16 +14127,16 @@
         <v>307</v>
       </c>
       <c r="E72" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F72" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G72" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H72" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -14144,7 +14144,7 @@
         <v>240</v>
       </c>
       <c r="B73" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C73" t="s">
         <v>243</v>
@@ -14153,16 +14153,16 @@
         <v>308</v>
       </c>
       <c r="E73" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F73" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G73" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H73" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -14170,7 +14170,7 @@
         <v>240</v>
       </c>
       <c r="B74" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C74" t="s">
         <v>243</v>
@@ -14179,16 +14179,16 @@
         <v>309</v>
       </c>
       <c r="E74" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F74" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G74" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H74" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -14196,7 +14196,7 @@
         <v>240</v>
       </c>
       <c r="B75" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C75" t="s">
         <v>243</v>
@@ -14205,16 +14205,16 @@
         <v>310</v>
       </c>
       <c r="E75" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F75" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G75" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H75" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -14222,7 +14222,7 @@
         <v>240</v>
       </c>
       <c r="B76" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C76" t="s">
         <v>243</v>
@@ -14231,16 +14231,16 @@
         <v>311</v>
       </c>
       <c r="E76" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F76" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G76" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H76" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -14248,7 +14248,7 @@
         <v>240</v>
       </c>
       <c r="B77" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C77" t="s">
         <v>243</v>
@@ -14257,16 +14257,16 @@
         <v>312</v>
       </c>
       <c r="E77" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F77" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G77" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H77" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -14274,7 +14274,7 @@
         <v>240</v>
       </c>
       <c r="B78" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C78" t="s">
         <v>243</v>
@@ -14283,16 +14283,16 @@
         <v>313</v>
       </c>
       <c r="E78" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F78" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G78" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H78" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -14300,7 +14300,7 @@
         <v>240</v>
       </c>
       <c r="B79" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C79" t="s">
         <v>243</v>
@@ -14309,16 +14309,16 @@
         <v>314</v>
       </c>
       <c r="E79" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F79" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G79" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H79" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -14326,7 +14326,7 @@
         <v>240</v>
       </c>
       <c r="B80" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C80" t="s">
         <v>243</v>
@@ -14335,16 +14335,16 @@
         <v>315</v>
       </c>
       <c r="E80" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F80" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G80" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H80" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -14352,7 +14352,7 @@
         <v>240</v>
       </c>
       <c r="B81" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C81" t="s">
         <v>243</v>
@@ -14361,16 +14361,16 @@
         <v>316</v>
       </c>
       <c r="E81" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F81" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G81" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H81" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -14378,7 +14378,7 @@
         <v>240</v>
       </c>
       <c r="B82" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C82" t="s">
         <v>243</v>
@@ -14387,16 +14387,16 @@
         <v>317</v>
       </c>
       <c r="E82" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F82" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G82" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H82" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -14404,7 +14404,7 @@
         <v>240</v>
       </c>
       <c r="B83" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C83" t="s">
         <v>243</v>
@@ -14413,16 +14413,16 @@
         <v>318</v>
       </c>
       <c r="E83" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F83" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G83" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H83" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -14430,7 +14430,7 @@
         <v>240</v>
       </c>
       <c r="B84" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C84" t="s">
         <v>243</v>
@@ -14439,16 +14439,16 @@
         <v>319</v>
       </c>
       <c r="E84" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F84" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G84" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H84" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -14456,7 +14456,7 @@
         <v>240</v>
       </c>
       <c r="B85" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C85" t="s">
         <v>243</v>
@@ -14465,16 +14465,16 @@
         <v>320</v>
       </c>
       <c r="E85" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F85" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G85" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H85" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -14482,7 +14482,7 @@
         <v>240</v>
       </c>
       <c r="B86" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C86" t="s">
         <v>243</v>
@@ -14491,16 +14491,16 @@
         <v>321</v>
       </c>
       <c r="E86" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F86" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G86" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H86" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -14508,7 +14508,7 @@
         <v>240</v>
       </c>
       <c r="B87" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C87" t="s">
         <v>243</v>
@@ -14517,16 +14517,16 @@
         <v>322</v>
       </c>
       <c r="E87" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F87" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G87" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H87" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -14534,7 +14534,7 @@
         <v>240</v>
       </c>
       <c r="B88" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C88" t="s">
         <v>243</v>
@@ -14543,16 +14543,16 @@
         <v>323</v>
       </c>
       <c r="E88" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F88" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G88" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H88" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -14560,7 +14560,7 @@
         <v>240</v>
       </c>
       <c r="B89" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C89" t="s">
         <v>243</v>
@@ -14569,16 +14569,16 @@
         <v>324</v>
       </c>
       <c r="E89" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F89" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G89" t="s">
-        <v>326</v>
+        <v>356</v>
       </c>
       <c r="H89" t="s">
-        <v>327</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>